<commit_message>
new version with co2 emission limit
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Investment in new capacity</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>(MtCO2)</t>
+  </si>
+  <si>
+    <t>additional CO2 price</t>
+  </si>
+  <si>
+    <t>(£/tCO2)</t>
   </si>
 </sst>
 </file>
@@ -593,16 +599,16 @@
         <v>0.0</v>
       </c>
       <c r="C5">
-        <v>225.14052135657175</v>
+        <v>803.9610370387693</v>
       </c>
       <c r="D5">
         <v>0.0</v>
       </c>
       <c r="E5">
-        <v>1629.3490875117495</v>
+        <v>1497.363716590231</v>
       </c>
       <c r="F5">
-        <v>1947.2639110843693</v>
+        <v>2297.9611550761024</v>
       </c>
       <c r="G5">
         <v>10000.0</v>
@@ -626,10 +632,10 @@
         <v>0.0</v>
       </c>
       <c r="O5">
-        <v>438.2088906345924</v>
+        <v>430.8730349492289</v>
       </c>
       <c r="P5">
-        <v>78.5671628927293</v>
+        <v>87.47013812979615</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -804,7 +810,7 @@
         <v>0.0</v>
       </c>
       <c r="C10">
-        <v>4824.286165362057</v>
+        <v>5960.562454366782</v>
       </c>
       <c r="D10">
         <v>0.0</v>
@@ -1009,16 +1015,16 @@
         <v>0.0</v>
       </c>
       <c r="C15">
-        <v>6668.3390397101</v>
+        <v>5705.43579468594</v>
       </c>
       <c r="D15">
-        <v>45.30266052180346</v>
+        <v>0.1330347427099241</v>
       </c>
       <c r="E15">
-        <v>1827.1910509473348</v>
+        <v>613.9063589030648</v>
       </c>
       <c r="F15">
-        <v>0.0</v>
+        <v>118.97250952878312</v>
       </c>
       <c r="G15">
         <v>0.0</v>
@@ -1036,7 +1042,7 @@
         <v>0.0</v>
       </c>
       <c r="L15">
-        <v>0.0</v>
+        <v>1.3300625785409543</v>
       </c>
       <c r="M15">
         <v>0.0</v>
@@ -1214,16 +1220,16 @@
         <v>0.0</v>
       </c>
       <c r="C20">
-        <v>4692.00343196606</v>
+        <v>3479.3746248175817</v>
       </c>
       <c r="D20">
-        <v>1546.898787636987</v>
+        <v>1038.9255100642702</v>
       </c>
       <c r="E20">
-        <v>3200.5557911873184</v>
+        <v>4395.68207624171</v>
       </c>
       <c r="F20">
-        <v>1596.64077129744</v>
+        <v>1744.8476670371006</v>
       </c>
       <c r="G20">
         <v>0.0</v>
@@ -1241,7 +1247,7 @@
         <v>0.0</v>
       </c>
       <c r="L20">
-        <v>18.700491345541877</v>
+        <v>3492.7931345445254</v>
       </c>
       <c r="M20">
         <v>0.0</v>
@@ -1416,19 +1422,19 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>0.0</v>
+        <v>127.98496165592496</v>
       </c>
       <c r="C25">
-        <v>3417.897840004229</v>
+        <v>3403.7662248724164</v>
       </c>
       <c r="D25">
-        <v>1447.467390725944</v>
+        <v>2461.268025575422</v>
       </c>
       <c r="E25">
-        <v>2238.621136808222</v>
+        <v>3188.614262169607</v>
       </c>
       <c r="F25">
-        <v>1168.4546109047778</v>
+        <v>1197.591562259594</v>
       </c>
       <c r="G25">
         <v>0.0</v>
@@ -1446,7 +1452,7 @@
         <v>3000.0</v>
       </c>
       <c r="L25">
-        <v>5302.539645951371</v>
+        <v>8865.59964266673</v>
       </c>
       <c r="M25">
         <v>0.0</v>
@@ -1627,13 +1633,13 @@
         <v>0.0</v>
       </c>
       <c r="D30">
-        <v>776.3660434875419</v>
+        <v>1234.925228422304</v>
       </c>
       <c r="E30">
-        <v>1741.3094144429942</v>
+        <v>940.3228063349052</v>
       </c>
       <c r="F30">
-        <v>3293.1999911762205</v>
+        <v>3607.424493376394</v>
       </c>
       <c r="G30">
         <v>0.0</v>
@@ -1651,7 +1657,7 @@
         <v>3000.0</v>
       </c>
       <c r="L30">
-        <v>4650.398329956358</v>
+        <v>9287.12563559234</v>
       </c>
       <c r="M30">
         <v>0.0</v>
@@ -1971,10 +1977,10 @@
         <v>5500.0</v>
       </c>
       <c r="O5">
-        <v>85.83183044232547</v>
+        <v>90.9513552166113</v>
       </c>
       <c r="P5">
-        <v>273.80989729953785</v>
+        <v>252.45154160282146</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1994,7 +2000,7 @@
         <v>17000.0</v>
       </c>
       <c r="F6">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G6">
         <v>5000.0</v>
@@ -2035,7 +2041,7 @@
         <v>17000.0</v>
       </c>
       <c r="F7">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G7">
         <v>5000.0</v>
@@ -2073,10 +2079,10 @@
         <v>5000.0</v>
       </c>
       <c r="E8">
-        <v>18629.34908751175</v>
+        <v>18497.363716590233</v>
       </c>
       <c r="F8">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G8">
         <v>5000.0</v>
@@ -2114,10 +2120,10 @@
         <v>5000.0</v>
       </c>
       <c r="E9">
-        <v>18629.34908751175</v>
+        <v>18497.363716590233</v>
       </c>
       <c r="F9">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G9">
         <v>5000.0</v>
@@ -2149,16 +2155,16 @@
         <v>10000.0</v>
       </c>
       <c r="C10">
-        <v>2225.1405213565718</v>
+        <v>2803.961037038769</v>
       </c>
       <c r="D10">
         <v>4000.0</v>
       </c>
       <c r="E10">
-        <v>17629.34908751175</v>
+        <v>17497.363716590233</v>
       </c>
       <c r="F10">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G10">
         <v>15000.0</v>
@@ -2190,16 +2196,16 @@
         <v>10000.0</v>
       </c>
       <c r="C11">
-        <v>2225.1405213565718</v>
+        <v>2803.961037038769</v>
       </c>
       <c r="D11">
         <v>4000.0</v>
       </c>
       <c r="E11">
-        <v>17629.34908751175</v>
+        <v>17497.363716590233</v>
       </c>
       <c r="F11">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G11">
         <v>15000.0</v>
@@ -2231,16 +2237,16 @@
         <v>10000.0</v>
       </c>
       <c r="C12">
-        <v>2225.1405213565718</v>
+        <v>2803.961037038769</v>
       </c>
       <c r="D12">
         <v>4000.0</v>
       </c>
       <c r="E12">
-        <v>17629.34908751175</v>
+        <v>17497.363716590233</v>
       </c>
       <c r="F12">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G12">
         <v>15000.0</v>
@@ -2272,16 +2278,16 @@
         <v>10000.0</v>
       </c>
       <c r="C13">
-        <v>2225.1405213565718</v>
+        <v>2803.961037038769</v>
       </c>
       <c r="D13">
         <v>4000.0</v>
       </c>
       <c r="E13">
-        <v>17629.34908751175</v>
+        <v>17497.363716590233</v>
       </c>
       <c r="F13">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G13">
         <v>15000.0</v>
@@ -2313,16 +2319,16 @@
         <v>10000.0</v>
       </c>
       <c r="C14">
-        <v>2225.1405213565718</v>
+        <v>2803.961037038769</v>
       </c>
       <c r="D14">
         <v>4000.0</v>
       </c>
       <c r="E14">
-        <v>17629.34908751175</v>
+        <v>17497.363716590233</v>
       </c>
       <c r="F14">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G14">
         <v>15000.0</v>
@@ -2354,16 +2360,16 @@
         <v>8000.0</v>
       </c>
       <c r="C15">
-        <v>7049.426686718629</v>
+        <v>8764.52349140555</v>
       </c>
       <c r="D15">
         <v>3500.0</v>
       </c>
       <c r="E15">
-        <v>15629.34908751175</v>
+        <v>15497.363716590231</v>
       </c>
       <c r="F15">
-        <v>2947.2639110843693</v>
+        <v>3297.9611550761024</v>
       </c>
       <c r="G15">
         <v>15000.0</v>
@@ -2395,16 +2401,16 @@
         <v>8000.0</v>
       </c>
       <c r="C16">
-        <v>7049.426686718629</v>
+        <v>8764.52349140555</v>
       </c>
       <c r="D16">
         <v>3500.0</v>
       </c>
       <c r="E16">
-        <v>15629.34908751175</v>
+        <v>15497.363716590231</v>
       </c>
       <c r="F16">
-        <v>2947.2639110843693</v>
+        <v>3416.9336646048855</v>
       </c>
       <c r="G16">
         <v>15000.0</v>
@@ -2436,16 +2442,16 @@
         <v>8000.0</v>
       </c>
       <c r="C17">
-        <v>7049.426686718629</v>
+        <v>8764.52349140555</v>
       </c>
       <c r="D17">
-        <v>3545.3026605218033</v>
+        <v>3500.13303474271</v>
       </c>
       <c r="E17">
-        <v>15629.34908751175</v>
+        <v>15497.363716590231</v>
       </c>
       <c r="F17">
-        <v>2947.2639110843693</v>
+        <v>3416.9336646048855</v>
       </c>
       <c r="G17">
         <v>15000.0</v>
@@ -2463,7 +2469,7 @@
         <v>25000.0</v>
       </c>
       <c r="L17">
-        <v>4100.0</v>
+        <v>4101.330062578541</v>
       </c>
       <c r="M17">
         <v>2500.0</v>
@@ -2477,16 +2483,16 @@
         <v>8000.0</v>
       </c>
       <c r="C18">
-        <v>7049.426686718629</v>
+        <v>8764.52349140555</v>
       </c>
       <c r="D18">
-        <v>3545.3026605218033</v>
+        <v>3500.13303474271</v>
       </c>
       <c r="E18">
-        <v>17456.540138459084</v>
+        <v>16111.270075493296</v>
       </c>
       <c r="F18">
-        <v>2947.2639110843693</v>
+        <v>3416.9336646048855</v>
       </c>
       <c r="G18">
         <v>15000.0</v>
@@ -2504,7 +2510,7 @@
         <v>25000.0</v>
       </c>
       <c r="L18">
-        <v>4100.0</v>
+        <v>4101.330062578541</v>
       </c>
       <c r="M18">
         <v>2500.0</v>
@@ -2518,16 +2524,16 @@
         <v>8000.0</v>
       </c>
       <c r="C19">
-        <v>7049.426686718629</v>
+        <v>8764.52349140555</v>
       </c>
       <c r="D19">
-        <v>3545.3026605218033</v>
+        <v>3500.13303474271</v>
       </c>
       <c r="E19">
-        <v>17456.540138459084</v>
+        <v>16111.270075493296</v>
       </c>
       <c r="F19">
-        <v>2947.2639110843693</v>
+        <v>3416.9336646048855</v>
       </c>
       <c r="G19">
         <v>15000.0</v>
@@ -2545,7 +2551,7 @@
         <v>25000.0</v>
       </c>
       <c r="L19">
-        <v>4100.0</v>
+        <v>4101.330062578541</v>
       </c>
       <c r="M19">
         <v>2500.0</v>
@@ -2559,16 +2565,16 @@
         <v>6000.0</v>
       </c>
       <c r="C20">
-        <v>13717.765726428728</v>
+        <v>14469.95928609149</v>
       </c>
       <c r="D20">
-        <v>2545.3026605218033</v>
+        <v>2500.13303474271</v>
       </c>
       <c r="E20">
-        <v>13456.540138459084</v>
+        <v>12111.270075493296</v>
       </c>
       <c r="F20">
-        <v>1947.2639110843693</v>
+        <v>2416.9336646048855</v>
       </c>
       <c r="G20">
         <v>15000.0</v>
@@ -2586,7 +2592,7 @@
         <v>25000.0</v>
       </c>
       <c r="L20">
-        <v>4100.0</v>
+        <v>4101.330062578541</v>
       </c>
       <c r="M20">
         <v>0.0</v>
@@ -2600,16 +2606,16 @@
         <v>6000.0</v>
       </c>
       <c r="C21">
-        <v>13717.765726428728</v>
+        <v>14469.95928609149</v>
       </c>
       <c r="D21">
-        <v>2545.3026605218033</v>
+        <v>2500.13303474271</v>
       </c>
       <c r="E21">
-        <v>13456.540138459084</v>
+        <v>12111.270075493296</v>
       </c>
       <c r="F21">
-        <v>3543.9046823818094</v>
+        <v>4161.781331641986</v>
       </c>
       <c r="G21">
         <v>15000.0</v>
@@ -2627,7 +2633,7 @@
         <v>25000.0</v>
       </c>
       <c r="L21">
-        <v>4100.0</v>
+        <v>4101.330062578541</v>
       </c>
       <c r="M21">
         <v>0.0</v>
@@ -2641,16 +2647,16 @@
         <v>6000.0</v>
       </c>
       <c r="C22">
-        <v>13717.765726428728</v>
+        <v>14469.95928609149</v>
       </c>
       <c r="D22">
-        <v>4092.2014481587903</v>
+        <v>3539.0585448069805</v>
       </c>
       <c r="E22">
-        <v>13456.540138459084</v>
+        <v>12111.270075493296</v>
       </c>
       <c r="F22">
-        <v>3543.9046823818094</v>
+        <v>4161.781331641986</v>
       </c>
       <c r="G22">
         <v>15000.0</v>
@@ -2668,7 +2674,7 @@
         <v>25000.0</v>
       </c>
       <c r="L22">
-        <v>4118.700491345542</v>
+        <v>7594.123197123066</v>
       </c>
       <c r="M22">
         <v>0.0</v>
@@ -2682,16 +2688,16 @@
         <v>6000.0</v>
       </c>
       <c r="C23">
-        <v>13717.765726428728</v>
+        <v>14469.95928609149</v>
       </c>
       <c r="D23">
-        <v>4092.2014481587903</v>
+        <v>3539.0585448069805</v>
       </c>
       <c r="E23">
-        <v>16657.095929646403</v>
+        <v>16506.952151735008</v>
       </c>
       <c r="F23">
-        <v>3543.9046823818094</v>
+        <v>4161.781331641986</v>
       </c>
       <c r="G23">
         <v>15000.0</v>
@@ -2709,7 +2715,7 @@
         <v>25000.0</v>
       </c>
       <c r="L23">
-        <v>4118.700491345542</v>
+        <v>7594.123197123066</v>
       </c>
       <c r="M23">
         <v>0.0</v>
@@ -2723,16 +2729,16 @@
         <v>6000.0</v>
       </c>
       <c r="C24">
-        <v>13717.765726428728</v>
+        <v>14469.95928609149</v>
       </c>
       <c r="D24">
-        <v>4092.2014481587903</v>
+        <v>3539.0585448069805</v>
       </c>
       <c r="E24">
-        <v>16657.095929646403</v>
+        <v>16506.952151735008</v>
       </c>
       <c r="F24">
-        <v>3543.9046823818094</v>
+        <v>4161.781331641986</v>
       </c>
       <c r="G24">
         <v>15000.0</v>
@@ -2750,7 +2756,7 @@
         <v>25000.0</v>
       </c>
       <c r="L24">
-        <v>4118.700491345542</v>
+        <v>7594.123197123066</v>
       </c>
       <c r="M24">
         <v>0.0</v>
@@ -2764,16 +2770,16 @@
         <v>5000.0</v>
       </c>
       <c r="C25">
-        <v>18409.769158394785</v>
+        <v>17949.333910909074</v>
       </c>
       <c r="D25">
-        <v>2592.2014481587903</v>
+        <v>2039.05854480698</v>
       </c>
       <c r="E25">
-        <v>13657.095929646403</v>
+        <v>13506.952151735006</v>
       </c>
       <c r="F25">
-        <v>3543.9046823818094</v>
+        <v>4161.781331641986</v>
       </c>
       <c r="G25">
         <v>15000.0</v>
@@ -2791,7 +2797,7 @@
         <v>22000.0</v>
       </c>
       <c r="L25">
-        <v>4118.700491345542</v>
+        <v>7594.123197123066</v>
       </c>
       <c r="M25">
         <v>0.0</v>
@@ -2805,16 +2811,16 @@
         <v>5000.0</v>
       </c>
       <c r="C26">
-        <v>18409.769158394785</v>
+        <v>17949.333910909074</v>
       </c>
       <c r="D26">
-        <v>2592.2014481587903</v>
+        <v>2039.05854480698</v>
       </c>
       <c r="E26">
-        <v>13657.095929646403</v>
+        <v>13506.952151735006</v>
       </c>
       <c r="F26">
-        <v>4712.359293286587</v>
+        <v>5359.37289390158</v>
       </c>
       <c r="G26">
         <v>15000.0</v>
@@ -2832,7 +2838,7 @@
         <v>25000.0</v>
       </c>
       <c r="L26">
-        <v>4118.700491345542</v>
+        <v>7594.123197123066</v>
       </c>
       <c r="M26">
         <v>0.0</v>
@@ -2846,16 +2852,16 @@
         <v>5000.0</v>
       </c>
       <c r="C27">
-        <v>18409.769158394785</v>
+        <v>17949.333910909074</v>
       </c>
       <c r="D27">
-        <v>4039.668838884734</v>
+        <v>4500.326570382402</v>
       </c>
       <c r="E27">
-        <v>13657.095929646403</v>
+        <v>13506.952151735006</v>
       </c>
       <c r="F27">
-        <v>4712.359293286587</v>
+        <v>5359.37289390158</v>
       </c>
       <c r="G27">
         <v>15000.0</v>
@@ -2873,7 +2879,7 @@
         <v>25000.0</v>
       </c>
       <c r="L27">
-        <v>9421.240137296914</v>
+        <v>16459.722839789796</v>
       </c>
       <c r="M27">
         <v>0.0</v>
@@ -2887,16 +2893,16 @@
         <v>5000.0</v>
       </c>
       <c r="C28">
-        <v>18409.769158394785</v>
+        <v>17949.333910909074</v>
       </c>
       <c r="D28">
-        <v>4039.668838884734</v>
+        <v>4500.326570382402</v>
       </c>
       <c r="E28">
-        <v>15895.717066454625</v>
+        <v>16695.566413904613</v>
       </c>
       <c r="F28">
-        <v>4712.359293286587</v>
+        <v>5359.37289390158</v>
       </c>
       <c r="G28">
         <v>15000.0</v>
@@ -2914,7 +2920,7 @@
         <v>25000.0</v>
       </c>
       <c r="L28">
-        <v>9421.240137296914</v>
+        <v>16459.722839789796</v>
       </c>
       <c r="M28">
         <v>0.0</v>
@@ -2928,16 +2934,16 @@
         <v>5000.0</v>
       </c>
       <c r="C29">
-        <v>18409.769158394785</v>
+        <v>17949.333910909074</v>
       </c>
       <c r="D29">
-        <v>4039.668838884734</v>
+        <v>4500.326570382402</v>
       </c>
       <c r="E29">
-        <v>15895.717066454625</v>
+        <v>16695.566413904613</v>
       </c>
       <c r="F29">
-        <v>4712.359293286587</v>
+        <v>5359.37289390158</v>
       </c>
       <c r="G29">
         <v>15000.0</v>
@@ -2955,7 +2961,7 @@
         <v>25000.0</v>
       </c>
       <c r="L29">
-        <v>9421.240137296914</v>
+        <v>16459.722839789796</v>
       </c>
       <c r="M29">
         <v>0.0</v>
@@ -2966,19 +2972,19 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>4000.0</v>
+        <v>4127.984961655925</v>
       </c>
       <c r="C30">
-        <v>21827.666998399014</v>
+        <v>21353.10013578149</v>
       </c>
       <c r="D30">
-        <v>4039.668838884734</v>
+        <v>4500.326570382402</v>
       </c>
       <c r="E30">
-        <v>13895.717066454625</v>
+        <v>14695.566413904613</v>
       </c>
       <c r="F30">
-        <v>4712.359293286587</v>
+        <v>5359.37289390158</v>
       </c>
       <c r="G30">
         <v>15000.0</v>
@@ -2996,7 +3002,7 @@
         <v>22000.0</v>
       </c>
       <c r="L30">
-        <v>9421.240137296914</v>
+        <v>16459.722839789796</v>
       </c>
       <c r="M30">
         <v>0.0</v>
@@ -3007,19 +3013,19 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>4000.0</v>
+        <v>4127.984961655925</v>
       </c>
       <c r="C31">
-        <v>21827.666998399014</v>
+        <v>21353.10013578149</v>
       </c>
       <c r="D31">
-        <v>4039.668838884734</v>
+        <v>4500.326570382402</v>
       </c>
       <c r="E31">
-        <v>13895.717066454625</v>
+        <v>14695.566413904613</v>
       </c>
       <c r="F31">
-        <v>6058.295373378438</v>
+        <v>6668.836232201871</v>
       </c>
       <c r="G31">
         <v>15000.0</v>
@@ -3037,7 +3043,7 @@
         <v>25000.0</v>
       </c>
       <c r="L31">
-        <v>9421.240137296914</v>
+        <v>16459.722839789796</v>
       </c>
       <c r="M31">
         <v>0.0</v>
@@ -3048,19 +3054,19 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>4000.0</v>
+        <v>4127.984961655925</v>
       </c>
       <c r="C32">
-        <v>21827.666998399014</v>
+        <v>21353.10013578149</v>
       </c>
       <c r="D32">
-        <v>4816.034882372276</v>
+        <v>5735.251798804706</v>
       </c>
       <c r="E32">
-        <v>13895.717066454625</v>
+        <v>14695.566413904613</v>
       </c>
       <c r="F32">
-        <v>6058.295373378438</v>
+        <v>6668.836232201871</v>
       </c>
       <c r="G32">
         <v>15000.0</v>
@@ -3078,7 +3084,7 @@
         <v>25000.0</v>
       </c>
       <c r="L32">
-        <v>14071.638467253273</v>
+        <v>25746.848475382136</v>
       </c>
       <c r="M32">
         <v>0.0</v>
@@ -3089,19 +3095,19 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>4000.0</v>
+        <v>4127.984961655925</v>
       </c>
       <c r="C33">
-        <v>21827.666998399014</v>
+        <v>21353.10013578149</v>
       </c>
       <c r="D33">
-        <v>4816.034882372276</v>
+        <v>5735.251798804706</v>
       </c>
       <c r="E33">
-        <v>15637.026480897619</v>
+        <v>15635.889220239518</v>
       </c>
       <c r="F33">
-        <v>6058.295373378438</v>
+        <v>6668.836232201871</v>
       </c>
       <c r="G33">
         <v>15000.0</v>
@@ -3119,7 +3125,7 @@
         <v>25000.0</v>
       </c>
       <c r="L33">
-        <v>14071.638467253273</v>
+        <v>25746.848475382136</v>
       </c>
       <c r="M33">
         <v>0.0</v>
@@ -3130,19 +3136,19 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>4000.0</v>
+        <v>4127.984961655925</v>
       </c>
       <c r="C34">
-        <v>21827.666998399014</v>
+        <v>21353.10013578149</v>
       </c>
       <c r="D34">
-        <v>4816.034882372276</v>
+        <v>5735.251798804706</v>
       </c>
       <c r="E34">
-        <v>15637.026480897619</v>
+        <v>15635.889220239518</v>
       </c>
       <c r="F34">
-        <v>6058.295373378438</v>
+        <v>6668.836232201871</v>
       </c>
       <c r="G34">
         <v>15000.0</v>
@@ -3160,7 +3166,7 @@
         <v>25000.0</v>
       </c>
       <c r="L34">
-        <v>14071.638467253273</v>
+        <v>25746.848475382136</v>
       </c>
       <c r="M34">
         <v>0.0</v>
@@ -3232,16 +3238,16 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>28.881490060422315</v>
+        <v>11.492883591785887</v>
       </c>
       <c r="C5">
         <v>17.52</v>
       </c>
       <c r="D5">
-        <v>2.165787847051109</v>
+        <v>19.554394315687563</v>
       </c>
       <c r="E5">
-        <v>135.2919979479179</v>
+        <v>135.291997947918</v>
       </c>
       <c r="F5">
         <v>0.16042972465095315</v>
@@ -3255,22 +3261,22 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>4.4666843035998065</v>
+        <v>4.466684303599806</v>
       </c>
       <c r="C6">
-        <v>16.949409595150183</v>
+        <v>16.93627944966481</v>
       </c>
       <c r="D6">
-        <v>9.118101501871482</v>
+        <v>9.118101501871484</v>
       </c>
       <c r="E6">
-        <v>104.87219989528525</v>
+        <v>104.8681725408936</v>
       </c>
       <c r="F6">
-        <v>0.08183996640567649</v>
+        <v>0.08569427441655028</v>
       </c>
       <c r="G6">
-        <v>43.18519258872348</v>
+        <v>43.213410482922974</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3278,22 +3284,22 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>4.773043142570227</v>
+        <v>4.773043142570225</v>
       </c>
       <c r="C7">
-        <v>16.980308513982237</v>
+        <v>16.965512606351798</v>
       </c>
       <c r="D7">
-        <v>9.563565943270218</v>
+        <v>9.563565943270225</v>
       </c>
       <c r="E7">
-        <v>106.0294422881765</v>
+        <v>106.02458186400393</v>
       </c>
       <c r="F7">
-        <v>0.09718406441686946</v>
+        <v>0.10154924242941013</v>
       </c>
       <c r="G7">
-        <v>43.2189709508588</v>
+        <v>43.25139344695766</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3301,22 +3307,22 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>3.4959753380930096</v>
+        <v>3.6091104630643396</v>
       </c>
       <c r="C8">
-        <v>17.002951622310526</v>
+        <v>16.99413825295042</v>
       </c>
       <c r="D8">
-        <v>7.3856785228706245</v>
+        <v>7.575360306197158</v>
       </c>
       <c r="E8">
-        <v>111.45594868926808</v>
+        <v>111.14657040704283</v>
       </c>
       <c r="F8">
-        <v>0.04552872471391029</v>
+        <v>0.05196259375661242</v>
       </c>
       <c r="G8">
-        <v>43.26389659853734</v>
+        <v>43.28396537132581</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3324,22 +3330,22 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>3.7561509271537665</v>
+        <v>3.876107114241729</v>
       </c>
       <c r="C9">
-        <v>17.03053505408529</v>
+        <v>17.020722131937312</v>
       </c>
       <c r="D9">
-        <v>7.761339908275128</v>
+        <v>7.955245815480021</v>
       </c>
       <c r="E9">
-        <v>112.74356850563218</v>
+        <v>112.42186728433019</v>
       </c>
       <c r="F9">
-        <v>0.05832618713486245</v>
+        <v>0.06575920517584274</v>
       </c>
       <c r="G9">
-        <v>43.291682735707354</v>
+        <v>43.31528588228263</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3347,22 +3353,22 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>0.35693800130581366</v>
+        <v>0.2940447868105326</v>
       </c>
       <c r="C10">
-        <v>14.965298051112391</v>
+        <v>18.507707231488595</v>
       </c>
       <c r="D10">
-        <v>1.0101931122213372</v>
+        <v>0.9028431216665117</v>
       </c>
       <c r="E10">
-        <v>48.16540573661014</v>
+        <v>44.78879543618919</v>
       </c>
       <c r="F10">
         <v>0.0</v>
       </c>
       <c r="G10">
-        <v>123.07201586844624</v>
+        <v>123.08810613967549</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3370,22 +3376,22 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>0.4093642574602117</v>
+        <v>0.3408855177021206</v>
       </c>
       <c r="C11">
-        <v>15.121506604607085</v>
+        <v>18.703905840146255</v>
       </c>
       <c r="D11">
-        <v>1.088834073219056</v>
+        <v>0.9768771413804677</v>
       </c>
       <c r="E11">
-        <v>49.54972029008454</v>
+        <v>46.1435047138381</v>
       </c>
       <c r="F11">
         <v>0.0</v>
       </c>
       <c r="G11">
-        <v>123.396178527097</v>
+        <v>123.40859733185158</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3393,22 +3399,22 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>0.46670750307311165</v>
+        <v>0.39152666213244414</v>
       </c>
       <c r="C12">
-        <v>15.260128167239321</v>
+        <v>18.897014999683062</v>
       </c>
       <c r="D12">
-        <v>1.17108254105681</v>
+        <v>1.054937855012834</v>
       </c>
       <c r="E12">
-        <v>50.945113634137655</v>
+        <v>47.505838050719596</v>
       </c>
       <c r="F12">
         <v>0.0</v>
       </c>
       <c r="G12">
-        <v>123.72158274541654</v>
+        <v>123.71627959750774</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3416,22 +3422,22 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>0.526567025160653</v>
+        <v>0.44749591137700834</v>
       </c>
       <c r="C13">
-        <v>15.408961717454787</v>
+        <v>19.091363557008886</v>
       </c>
       <c r="D13">
-        <v>1.25917806844019</v>
+        <v>1.133210897698477</v>
       </c>
       <c r="E13">
-        <v>52.34754801851635</v>
+        <v>48.877377742168996</v>
       </c>
       <c r="F13">
         <v>0.0</v>
       </c>
       <c r="G13">
-        <v>124.01518963246852</v>
+        <v>124.00897401924342</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3439,22 +3445,22 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>0.5891347056941215</v>
+        <v>0.506219216620154</v>
       </c>
       <c r="C14">
-        <v>15.54836639548465</v>
+        <v>19.27818156869697</v>
       </c>
       <c r="D14">
-        <v>1.3551335829625106</v>
+        <v>1.2183007505103933</v>
       </c>
       <c r="E14">
-        <v>53.75548050917558</v>
+        <v>50.25655131062698</v>
       </c>
       <c r="F14">
         <v>0.0</v>
       </c>
       <c r="G14">
-        <v>124.30366663056235</v>
+        <v>124.29190629668412</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3462,22 +3468,22 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>0.287133911484479</v>
+        <v>0.12565968293048718</v>
       </c>
       <c r="C15">
-        <v>43.3708571446532</v>
+        <v>50.81425523761625</v>
       </c>
       <c r="D15">
-        <v>0.7077145718576312</v>
+        <v>0.47292002532360317</v>
       </c>
       <c r="E15">
-        <v>30.319169821099937</v>
+        <v>23.283198698344158</v>
       </c>
       <c r="F15">
-        <v>0.00022819016271726468</v>
+        <v>0.0</v>
       </c>
       <c r="G15">
-        <v>124.6713930394099</v>
+        <v>124.65998846716757</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3485,22 +3491,22 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>0.4350529868142453</v>
+        <v>0.2199326624499516</v>
       </c>
       <c r="C16">
-        <v>44.91252882673885</v>
+        <v>52.822172550077525</v>
       </c>
       <c r="D16">
-        <v>0.8955518881770752</v>
+        <v>0.5993594581927059</v>
       </c>
       <c r="E16">
-        <v>33.659899631224995</v>
+        <v>26.280665311932434</v>
       </c>
       <c r="F16">
-        <v>0.0014661593859215244</v>
+        <v>0.0</v>
       </c>
       <c r="G16">
-        <v>125.43833358832424</v>
+        <v>125.41970654069635</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3508,22 +3514,22 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>0.6032026776589853</v>
+        <v>0.34779517554800077</v>
       </c>
       <c r="C17">
-        <v>46.33766880195652</v>
+        <v>54.713878893938094</v>
       </c>
       <c r="D17">
-        <v>1.1250012664546745</v>
+        <v>0.7646360894632591</v>
       </c>
       <c r="E17">
-        <v>37.12861048389635</v>
+        <v>29.39258740252358</v>
       </c>
       <c r="F17">
-        <v>0.005608686148455528</v>
+        <v>0.0008497639380650798</v>
       </c>
       <c r="G17">
-        <v>126.12769736431638</v>
+        <v>126.10464244327521</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3531,22 +3537,22 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>0.4584945161346475</v>
+        <v>0.4071133473143775</v>
       </c>
       <c r="C18">
-        <v>47.65899188623381</v>
+        <v>56.491424925096574</v>
       </c>
       <c r="D18">
-        <v>0.9134168294105245</v>
+        <v>0.8289308088779457</v>
       </c>
       <c r="E18">
-        <v>41.526768030874436</v>
+        <v>32.85164314738478</v>
       </c>
       <c r="F18">
-        <v>0.002368445251355881</v>
+        <v>0.0014374478900305622</v>
       </c>
       <c r="G18">
-        <v>126.74951873363959</v>
+        <v>126.73260518048882</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3554,22 +3560,22 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>0.6352901002825088</v>
+        <v>0.3707287097746543</v>
       </c>
       <c r="C19">
-        <v>48.87251623931701</v>
+        <v>58.05228653175078</v>
       </c>
       <c r="D19">
-        <v>1.131559472567821</v>
+        <v>1.0349432274328414</v>
       </c>
       <c r="E19">
-        <v>45.34171070396893</v>
+        <v>36.2361280592374</v>
       </c>
       <c r="F19">
-        <v>0.00778782544093337</v>
+        <v>0.20804382571002197</v>
       </c>
       <c r="G19">
-        <v>127.3060569281972</v>
+        <v>127.55104333805646</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3577,22 +3583,22 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>0.5067628028861741</v>
+        <v>0.6150572816597963</v>
       </c>
       <c r="C20">
-        <v>82.30882234424232</v>
+        <v>84.86597384657841</v>
       </c>
       <c r="D20">
-        <v>0.6168332016651467</v>
+        <v>0.7077033559464845</v>
       </c>
       <c r="E20">
-        <v>20.18550050428116</v>
+        <v>17.41274450457653</v>
       </c>
       <c r="F20">
-        <v>0.021644933352451285</v>
+        <v>0.03175114172071534</v>
       </c>
       <c r="G20">
-        <v>127.88880230097169</v>
+        <v>127.88594847825674</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3600,22 +3606,22 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>0.6801283341795956</v>
+        <v>0.8074404428721602</v>
       </c>
       <c r="C21">
-        <v>84.9420266626021</v>
+        <v>87.69462949171029</v>
       </c>
       <c r="D21">
-        <v>0.7779090613914796</v>
+        <v>0.875628838708774</v>
       </c>
       <c r="E21">
-        <v>22.762662596695854</v>
+        <v>19.75454141474421</v>
       </c>
       <c r="F21">
-        <v>0.04491481432553155</v>
+        <v>0.06872614094560778</v>
       </c>
       <c r="G21">
-        <v>128.32039847886855</v>
+        <v>128.31918442008234</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3623,22 +3629,22 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>0.5809229390414411</v>
+        <v>0.6931861358509351</v>
       </c>
       <c r="C22">
-        <v>87.4202921722385</v>
+        <v>85.45472677200397</v>
       </c>
       <c r="D22">
-        <v>1.3042128190073108</v>
+        <v>1.1814940533187872</v>
       </c>
       <c r="E22">
-        <v>25.435610626101813</v>
+        <v>19.716366851267665</v>
       </c>
       <c r="F22">
-        <v>0.035430221095793114</v>
+        <v>0.05469378453261846</v>
       </c>
       <c r="G22">
-        <v>128.7019865022224</v>
+        <v>127.01091595292955</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3646,22 +3652,22 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>0.269955161398312</v>
+        <v>0.2184382022454988</v>
       </c>
       <c r="C23">
-        <v>89.79425211824606</v>
+        <v>88.11219246650508</v>
       </c>
       <c r="D23">
-        <v>0.788940902784412</v>
+        <v>0.5520130053113396</v>
       </c>
       <c r="E23">
-        <v>29.56601546497127</v>
+        <v>23.713716950925434</v>
       </c>
       <c r="F23">
-        <v>0.007338125715961147</v>
+        <v>0.005521805235611288</v>
       </c>
       <c r="G23">
-        <v>129.0484617446176</v>
+        <v>127.50235328685618</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3669,22 +3675,22 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>0.39821312530917297</v>
+        <v>0.05527045329263642</v>
       </c>
       <c r="C24">
-        <v>92.04542483856132</v>
+        <v>90.51216704854355</v>
       </c>
       <c r="D24">
-        <v>0.9763258962191245</v>
+        <v>0.6763092347771626</v>
       </c>
       <c r="E24">
-        <v>32.678101186434716</v>
+        <v>26.49392393780331</v>
       </c>
       <c r="F24">
-        <v>0.019687243910526776</v>
+        <v>0.2896965955153706</v>
       </c>
       <c r="G24">
-        <v>129.35369043566402</v>
+        <v>128.2668534024937</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3692,22 +3698,22 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>0.5632283621307705</v>
+        <v>0.6578403253678454</v>
       </c>
       <c r="C25">
-        <v>117.76662750229316</v>
+        <v>110.4281189656015</v>
       </c>
       <c r="D25">
-        <v>0.6855882876607637</v>
+        <v>0.5653556535364932</v>
       </c>
       <c r="E25">
-        <v>20.06332355338073</v>
+        <v>18.939209523738118</v>
       </c>
       <c r="F25">
-        <v>0.06345984839072787</v>
+        <v>0.09893865332712266</v>
       </c>
       <c r="G25">
-        <v>130.41264924629508</v>
+        <v>129.47351856736609</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3715,22 +3721,22 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>0.6426596562367495</v>
+        <v>0.6694893203272386</v>
       </c>
       <c r="C26">
-        <v>115.79408777077725</v>
+        <v>108.51071229196042</v>
       </c>
       <c r="D26">
-        <v>0.7449474383973964</v>
+        <v>0.6250204168273392</v>
       </c>
       <c r="E26">
-        <v>20.301560960070233</v>
+        <v>19.260235496935874</v>
       </c>
       <c r="F26">
-        <v>0.0985788357990431</v>
+        <v>0.20686617203133476</v>
       </c>
       <c r="G26">
-        <v>129.86969275760558</v>
+        <v>128.94106806442682</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3738,22 +3744,22 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>0.46932368004042374</v>
+        <v>0.36945367588515826</v>
       </c>
       <c r="C27">
-        <v>110.19120514129499</v>
+        <v>97.98824442881168</v>
       </c>
       <c r="D27">
-        <v>1.0033868645828978</v>
+        <v>0.9615308148654725</v>
       </c>
       <c r="E27">
-        <v>19.103480184723548</v>
+        <v>16.440722709630208</v>
       </c>
       <c r="F27">
-        <v>0.05801133140262328</v>
+        <v>0.043329207253469545</v>
       </c>
       <c r="G27">
-        <v>128.33298869006117</v>
+        <v>124.55843456153404</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3761,22 +3767,22 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>0.31263537033479083</v>
+        <v>0.1641257396295878</v>
       </c>
       <c r="C28">
-        <v>113.20454820759356</v>
+        <v>101.04955962996488</v>
       </c>
       <c r="D28">
-        <v>0.7694842359685872</v>
+        <v>0.6197987596311448</v>
       </c>
       <c r="E28">
-        <v>22.15608079258733</v>
+        <v>19.32201405204778</v>
       </c>
       <c r="F28">
-        <v>0.03344095162350312</v>
+        <v>0.01360647151942501</v>
       </c>
       <c r="G28">
-        <v>128.67955948727135</v>
+        <v>125.15459450583856</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3784,22 +3790,22 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>0.43818169433124177</v>
+        <v>0.2463989723960163</v>
       </c>
       <c r="C29">
-        <v>116.07817376844291</v>
+        <v>103.97959244998299</v>
       </c>
       <c r="D29">
-        <v>0.9330235213324298</v>
+        <v>0.7447715621741567</v>
       </c>
       <c r="E29">
-        <v>24.657025668868528</v>
+        <v>21.58052626476842</v>
       </c>
       <c r="F29">
-        <v>0.05436006592623207</v>
+        <v>0.02722792873808198</v>
       </c>
       <c r="G29">
-        <v>128.98881384911314</v>
+        <v>125.71381734875109</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3807,22 +3813,22 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>0.4065224698054191</v>
+        <v>0.23315476807001753</v>
       </c>
       <c r="C30">
-        <v>135.52251865703332</v>
+        <v>121.76233570730516</v>
       </c>
       <c r="D30">
-        <v>0.9409101088647566</v>
+        <v>0.7435644281929789</v>
       </c>
       <c r="E30">
-        <v>18.16714868512927</v>
+        <v>15.79284348013266</v>
       </c>
       <c r="F30">
-        <v>0.08968356802411005</v>
+        <v>0.03996719231544301</v>
       </c>
       <c r="G30">
-        <v>130.08594587027088</v>
+        <v>127.6768684546037</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3830,22 +3836,22 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>0.46859827735413784</v>
+        <v>0.29244119980296956</v>
       </c>
       <c r="C31">
-        <v>133.4988887098176</v>
+        <v>120.10535474019402</v>
       </c>
       <c r="D31">
-        <v>1.0175928621578605</v>
+        <v>0.8157988913877546</v>
       </c>
       <c r="E31">
-        <v>18.49496573650747</v>
+        <v>16.25655578158666</v>
       </c>
       <c r="F31">
-        <v>0.1277161200999193</v>
+        <v>0.05704788873147013</v>
       </c>
       <c r="G31">
-        <v>129.51358058196666</v>
+        <v>126.69353873777094</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3853,22 +3859,22 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>0.4166943534709609</v>
+        <v>0.1822120096995416</v>
       </c>
       <c r="C32">
-        <v>128.76165058004378</v>
+        <v>108.79061017906619</v>
       </c>
       <c r="D32">
-        <v>1.1698654842551035</v>
+        <v>0.8779363374162614</v>
       </c>
       <c r="E32">
-        <v>17.940129762535598</v>
+        <v>14.227133814343855</v>
       </c>
       <c r="F32">
-        <v>0.11522859724282808</v>
+        <v>0.03533505164498108</v>
       </c>
       <c r="G32">
-        <v>128.21014090368521</v>
+        <v>121.71398380438144</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3876,22 +3882,22 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>0.34190822775257534</v>
+        <v>0.18763864024522733</v>
       </c>
       <c r="C33">
-        <v>131.99796825286305</v>
+        <v>112.11826783211589</v>
       </c>
       <c r="D33">
-        <v>1.0071189316382083</v>
+        <v>0.8800234735964654</v>
       </c>
       <c r="E33">
-        <v>20.636915446694005</v>
+        <v>16.11469312033304</v>
       </c>
       <c r="F33">
-        <v>0.08396608571917372</v>
+        <v>0.037509785837174785</v>
       </c>
       <c r="G33">
-        <v>128.5360976548082</v>
+        <v>122.39954764386455</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3899,22 +3905,22 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>0.44507111058547943</v>
+        <v>0.011884189764610935</v>
       </c>
       <c r="C34">
-        <v>135.13099051504437</v>
+        <v>114.76083974792115</v>
       </c>
       <c r="D34">
-        <v>1.1975120048375738</v>
+        <v>1.04524386148472</v>
       </c>
       <c r="E34">
-        <v>22.85675963395058</v>
+        <v>17.897150236863475</v>
       </c>
       <c r="F34">
-        <v>0.13161620643709093</v>
+        <v>0.30219095009647945</v>
       </c>
       <c r="G34">
-        <v>128.8345124627154</v>
+        <v>124.58116385137428</v>
       </c>
     </row>
   </sheetData>
@@ -3983,22 +3989,22 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>0.8250588783617319</v>
+        <v>0.8259075909628004</v>
       </c>
       <c r="C5">
-        <v>0.22736658510418561</v>
+        <v>0.22651787250311695</v>
       </c>
       <c r="D5">
-        <v>0.21710788570615983</v>
+        <v>0.21710788570615977</v>
       </c>
       <c r="E5">
-        <v>0.6600471026893853</v>
+        <v>0.6607260727702401</v>
       </c>
       <c r="F5">
-        <v>0.1818932680833485</v>
+        <v>0.18121429800249356</v>
       </c>
       <c r="G5">
-        <v>0.19973925484966631</v>
+        <v>0.19973925484966626</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4006,22 +4012,22 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>0.6747346537676402</v>
+        <v>0.6748823930799471</v>
       </c>
       <c r="C6">
-        <v>0.18776723723531014</v>
+        <v>0.18786972518063333</v>
       </c>
       <c r="D6">
-        <v>0.19542159511594157</v>
+        <v>0.19560794505116855</v>
       </c>
       <c r="E6">
-        <v>0.539787723014112</v>
+        <v>0.5399059144639572</v>
       </c>
       <c r="F6">
-        <v>0.15021378978824815</v>
+        <v>0.15029578014450665</v>
       </c>
       <c r="G6">
-        <v>0.17978786750666578</v>
+        <v>0.17995930944707453</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4029,22 +4035,22 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>0.6823670831663776</v>
+        <v>0.6828658488885798</v>
       </c>
       <c r="C7">
-        <v>0.1908882958303402</v>
+        <v>0.19065956809491663</v>
       </c>
       <c r="D7">
-        <v>0.19884815038850898</v>
+        <v>0.1987916286493786</v>
       </c>
       <c r="E7">
-        <v>0.5458936665331015</v>
+        <v>0.5462926791108633</v>
       </c>
       <c r="F7">
-        <v>0.15271063666427215</v>
+        <v>0.15252765447593333</v>
       </c>
       <c r="G7">
-        <v>0.18294029835742784</v>
+        <v>0.18288829835742781</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4052,22 +4058,22 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>0.6037126030002785</v>
+        <v>0.6114972611212726</v>
       </c>
       <c r="C8">
-        <v>0.1722183648562327</v>
+        <v>0.1737092989249779</v>
       </c>
       <c r="D8">
-        <v>0.17932027112226034</v>
+        <v>0.18007870996834127</v>
       </c>
       <c r="E8">
-        <v>0.4829700824002229</v>
+        <v>0.48919780889701797</v>
       </c>
       <c r="F8">
-        <v>0.13777469188498612</v>
+        <v>0.13896743913998233</v>
       </c>
       <c r="G8">
-        <v>0.164974649432479</v>
+        <v>0.16567241317087347</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4075,22 +4081,22 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>0.6154667482328815</v>
+        <v>0.6241038555585505</v>
       </c>
       <c r="C9">
-        <v>0.17434003066081896</v>
+        <v>0.17619298287618362</v>
       </c>
       <c r="D9">
-        <v>0.18057370503217465</v>
+        <v>0.18290662134779262</v>
       </c>
       <c r="E9">
-        <v>0.49237339858630513</v>
+        <v>0.4992830844468405</v>
       </c>
       <c r="F9">
-        <v>0.13947202452865518</v>
+        <v>0.14095438630094695</v>
       </c>
       <c r="G9">
-        <v>0.1661278086296003</v>
+        <v>0.1682740916399688</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4098,22 +4104,22 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>0.6345221003296821</v>
+        <v>0.6621766181965069</v>
       </c>
       <c r="C10">
-        <v>0.17029850148382</v>
+        <v>0.18033639359553696</v>
       </c>
       <c r="D10">
-        <v>0.19196960200343408</v>
+        <v>0.19926567779867918</v>
       </c>
       <c r="E10">
-        <v>0.5076176802637458</v>
+        <v>0.5297412945572051</v>
       </c>
       <c r="F10">
-        <v>0.136238801187056</v>
+        <v>0.1442691148764296</v>
       </c>
       <c r="G10">
-        <v>0.1766120338431588</v>
+        <v>0.18332442357478435</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4121,22 +4127,22 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>0.6293712608814303</v>
+        <v>0.65324106023405</v>
       </c>
       <c r="C11">
-        <v>0.17082626766816053</v>
+        <v>0.17913051847439015</v>
       </c>
       <c r="D11">
-        <v>0.18893132713751307</v>
+        <v>0.1970145842621571</v>
       </c>
       <c r="E11">
-        <v>0.5034970087051444</v>
+        <v>0.52259284818724</v>
       </c>
       <c r="F11">
-        <v>0.13666101413452844</v>
+        <v>0.14330441477951208</v>
       </c>
       <c r="G11">
-        <v>0.17381682096651163</v>
+        <v>0.18125341752118404</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4144,22 +4150,22 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>0.6218093100684475</v>
+        <v>0.6446209341136002</v>
       </c>
       <c r="C12">
-        <v>0.17129218145102174</v>
+        <v>0.17782426480252486</v>
       </c>
       <c r="D12">
-        <v>0.18608347925800983</v>
+        <v>0.19499332250691945</v>
       </c>
       <c r="E12">
-        <v>0.497447448054758</v>
+        <v>0.5156967472908791</v>
       </c>
       <c r="F12">
-        <v>0.1370337451608174</v>
+        <v>0.14225941184201985</v>
       </c>
       <c r="G12">
-        <v>0.17119680091736855</v>
+        <v>0.1793938567063653</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4167,22 +4173,22 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>0.6144027142118422</v>
+        <v>0.6420999901690336</v>
       </c>
       <c r="C13">
-        <v>0.170044736337712</v>
+        <v>0.17678017724194325</v>
       </c>
       <c r="D13">
-        <v>0.1850671370478399</v>
+        <v>0.19320441137508843</v>
       </c>
       <c r="E13">
-        <v>0.4915221713694738</v>
+        <v>0.513679992135227</v>
       </c>
       <c r="F13">
-        <v>0.13603578907016958</v>
+        <v>0.1414241417935546</v>
       </c>
       <c r="G13">
-        <v>0.17026176608401217</v>
+        <v>0.17774805846508085</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4190,22 +4196,22 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>0.6081726852701885</v>
+        <v>0.6384395320411661</v>
       </c>
       <c r="C14">
-        <v>0.16814596446891802</v>
+        <v>0.17517716896542831</v>
       </c>
       <c r="D14">
-        <v>0.18303938632970623</v>
+        <v>0.18857122803882964</v>
       </c>
       <c r="E14">
-        <v>0.4865381482161507</v>
+        <v>0.5107516256329329</v>
       </c>
       <c r="F14">
-        <v>0.13451677157513442</v>
+        <v>0.14014173517234266</v>
       </c>
       <c r="G14">
-        <v>0.1683962354233292</v>
+        <v>0.17348552979572274</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4213,19 +4219,19 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>0.8434854271849384</v>
+        <v>0.8641288939322233</v>
       </c>
       <c r="C15">
-        <v>0.23028893400409395</v>
+        <v>0.23744776628839345</v>
       </c>
       <c r="D15">
         <v>0.0</v>
       </c>
       <c r="E15">
-        <v>0.6747883417479497</v>
+        <v>0.6913031151457776</v>
       </c>
       <c r="F15">
-        <v>0.1842311472032752</v>
+        <v>0.18995821303071472</v>
       </c>
       <c r="G15">
         <v>0.0</v>
@@ -4236,19 +4242,19 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>0.8196813254581796</v>
+        <v>0.8565519080364377</v>
       </c>
       <c r="C16">
-        <v>0.22631955927918201</v>
+        <v>0.24042779708999074</v>
       </c>
       <c r="D16">
         <v>0.0</v>
       </c>
       <c r="E16">
-        <v>0.6557450603665441</v>
+        <v>0.6852415264291504</v>
       </c>
       <c r="F16">
-        <v>0.18105564742334568</v>
+        <v>0.19234223767199263</v>
       </c>
       <c r="G16">
         <v>0.0</v>
@@ -4259,19 +4265,19 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>0.799863016244524</v>
+        <v>0.8487825561641716</v>
       </c>
       <c r="C17">
-        <v>0.2190531578919215</v>
+        <v>0.23771996577023383</v>
       </c>
       <c r="D17">
         <v>0.0</v>
       </c>
       <c r="E17">
-        <v>0.6398904129956194</v>
+        <v>0.679026044931337</v>
       </c>
       <c r="F17">
-        <v>0.17524252631353718</v>
+        <v>0.19017597261618696</v>
       </c>
       <c r="G17">
         <v>0.0</v>
@@ -4282,19 +4288,19 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>0.7630083096904691</v>
+        <v>0.8349836105812825</v>
       </c>
       <c r="C18">
-        <v>0.20875263702698482</v>
+        <v>0.22926117002454913</v>
       </c>
       <c r="D18">
         <v>0.0</v>
       </c>
       <c r="E18">
-        <v>0.6104066477523755</v>
+        <v>0.6679868884650262</v>
       </c>
       <c r="F18">
-        <v>0.16700210962158785</v>
+        <v>0.1834089360196393</v>
       </c>
       <c r="G18">
         <v>0.0</v>
@@ -4305,19 +4311,19 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>0.7387324210731044</v>
+        <v>0.8199521616490035</v>
       </c>
       <c r="C19">
-        <v>0.20126642514348048</v>
+        <v>0.22549570778354974</v>
       </c>
       <c r="D19">
         <v>0.0</v>
       </c>
       <c r="E19">
-        <v>0.5909859368584833</v>
+        <v>0.655961729319203</v>
       </c>
       <c r="F19">
-        <v>0.16101314011478438</v>
+        <v>0.1803965662268398</v>
       </c>
       <c r="G19">
         <v>0.0</v>
@@ -4328,19 +4334,19 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>0.8143280870032342</v>
+        <v>0.8000321797737816</v>
       </c>
       <c r="C20">
-        <v>0.23067032776145058</v>
+        <v>0.2241706766648045</v>
       </c>
       <c r="D20">
         <v>0.0</v>
       </c>
       <c r="E20">
-        <v>0.6514624696025878</v>
+        <v>0.640025743819025</v>
       </c>
       <c r="F20">
-        <v>0.18453626220916056</v>
+        <v>0.17933654133184362</v>
       </c>
       <c r="G20">
         <v>0.0</v>
@@ -4351,19 +4357,19 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>0.8238546249585981</v>
+        <v>0.8068460007942442</v>
       </c>
       <c r="C21">
-        <v>0.23321282929576664</v>
+        <v>0.22959522970623192</v>
       </c>
       <c r="D21">
         <v>0.0</v>
       </c>
       <c r="E21">
-        <v>0.6590836999668784</v>
+        <v>0.6454768006353951</v>
       </c>
       <c r="F21">
-        <v>0.18657026343661332</v>
+        <v>0.1836761837649856</v>
       </c>
       <c r="G21">
         <v>0.0</v>
@@ -4374,19 +4380,19 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>0.8354688683799862</v>
+        <v>0.8166008966229649</v>
       </c>
       <c r="C22">
-        <v>0.23417966727398862</v>
+        <v>0.22960005712564607</v>
       </c>
       <c r="D22">
         <v>0.0</v>
       </c>
       <c r="E22">
-        <v>0.668375094703989</v>
+        <v>0.6532807172983722</v>
       </c>
       <c r="F22">
-        <v>0.1873437338191909</v>
+        <v>0.18368004570051688</v>
       </c>
       <c r="G22">
         <v>0.0</v>
@@ -4397,19 +4403,19 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>0.8304257756539132</v>
+        <v>0.8125012060105963</v>
       </c>
       <c r="C23">
-        <v>0.2313065830446203</v>
+        <v>0.2296818938655498</v>
       </c>
       <c r="D23">
         <v>0.0</v>
       </c>
       <c r="E23">
-        <v>0.6643406205231303</v>
+        <v>0.6500009648084766</v>
       </c>
       <c r="F23">
-        <v>0.18504526643569622</v>
+        <v>0.1837455150924399</v>
       </c>
       <c r="G23">
         <v>0.0</v>
@@ -4420,19 +4426,19 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>0.8281586110077267</v>
+        <v>0.8266413766620692</v>
       </c>
       <c r="C24">
-        <v>0.22950217750941068</v>
+        <v>0.23391801369427076</v>
       </c>
       <c r="D24">
         <v>0.0</v>
       </c>
       <c r="E24">
-        <v>0.6625268888061813</v>
+        <v>0.6613131013296554</v>
       </c>
       <c r="F24">
-        <v>0.18360174200752857</v>
+        <v>0.18713441095541658</v>
       </c>
       <c r="G24">
         <v>0.0</v>
@@ -4443,19 +4449,19 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>0.7565974432665419</v>
+        <v>0.7625429331753633</v>
       </c>
       <c r="C25">
-        <v>0.22110718283377628</v>
+        <v>0.21808131287643545</v>
       </c>
       <c r="D25">
         <v>0.0</v>
       </c>
       <c r="E25">
-        <v>0.6052779546132333</v>
+        <v>0.610034346540291</v>
       </c>
       <c r="F25">
-        <v>0.176885746267021</v>
+        <v>0.17446505030114834</v>
       </c>
       <c r="G25">
         <v>0.0</v>
@@ -4466,19 +4472,19 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>0.7629932593641368</v>
+        <v>0.7816674703950781</v>
       </c>
       <c r="C26">
-        <v>0.22122651155001402</v>
+        <v>0.2214252639949303</v>
       </c>
       <c r="D26">
         <v>0.0</v>
       </c>
       <c r="E26">
-        <v>0.6103946074913092</v>
+        <v>0.6253339763160626</v>
       </c>
       <c r="F26">
-        <v>0.17698120924001126</v>
+        <v>0.17714021119594417</v>
       </c>
       <c r="G26">
         <v>0.0</v>
@@ -4489,19 +4495,19 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>0.7727759898174179</v>
+        <v>0.7818843606322876</v>
       </c>
       <c r="C27">
-        <v>0.2179581231250782</v>
+        <v>0.21883212180829553</v>
       </c>
       <c r="D27">
         <v>0.0</v>
       </c>
       <c r="E27">
-        <v>0.6182207918539343</v>
+        <v>0.6255074885058304</v>
       </c>
       <c r="F27">
-        <v>0.17436649850006253</v>
+        <v>0.17506569744663641</v>
       </c>
       <c r="G27">
         <v>0.0</v>
@@ -4512,19 +4518,19 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>0.7826486441384227</v>
+        <v>0.7865513460989046</v>
       </c>
       <c r="C28">
-        <v>0.22424761920914862</v>
+        <v>0.22005722929134447</v>
       </c>
       <c r="D28">
         <v>0.0</v>
       </c>
       <c r="E28">
-        <v>0.626118915310738</v>
+        <v>0.6292410768791237</v>
       </c>
       <c r="F28">
-        <v>0.17939809536731885</v>
+        <v>0.17604578343307553</v>
       </c>
       <c r="G28">
         <v>0.0</v>
@@ -4535,19 +4541,19 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>0.788619150966516</v>
+        <v>0.7885648718901332</v>
       </c>
       <c r="C29">
-        <v>0.2263413774955616</v>
+        <v>0.22106920029475938</v>
       </c>
       <c r="D29">
         <v>0.0</v>
       </c>
       <c r="E29">
-        <v>0.6308953207732129</v>
+        <v>0.6308518975121068</v>
       </c>
       <c r="F29">
-        <v>0.18107310199644935</v>
+        <v>0.17685536023580742</v>
       </c>
       <c r="G29">
         <v>0.0</v>
@@ -4558,19 +4564,19 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>0.7193545501509547</v>
+        <v>0.7073780219392636</v>
       </c>
       <c r="C30">
-        <v>0.20988646060983845</v>
+        <v>0.19910573823236213</v>
       </c>
       <c r="D30">
         <v>0.0</v>
       </c>
       <c r="E30">
-        <v>0.5754836401207629</v>
+        <v>0.5659024175514107</v>
       </c>
       <c r="F30">
-        <v>0.16790916848787077</v>
+        <v>0.1592845905858897</v>
       </c>
       <c r="G30">
         <v>0.0</v>
@@ -4581,19 +4587,19 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>0.7243222272386866</v>
+        <v>0.7195361832929923</v>
       </c>
       <c r="C31">
-        <v>0.2099524585126309</v>
+        <v>0.2032313549441349</v>
       </c>
       <c r="D31">
         <v>0.0</v>
       </c>
       <c r="E31">
-        <v>0.5794577817909492</v>
+        <v>0.5756289466343938</v>
       </c>
       <c r="F31">
-        <v>0.16796196681010472</v>
+        <v>0.1625850839553079</v>
       </c>
       <c r="G31">
         <v>0.0</v>
@@ -4604,19 +4610,19 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>0.7372128380532128</v>
+        <v>0.7299894929446618</v>
       </c>
       <c r="C32">
-        <v>0.2089902435250931</v>
+        <v>0.20253676582025232</v>
       </c>
       <c r="D32">
         <v>0.0</v>
       </c>
       <c r="E32">
-        <v>0.5897702704425705</v>
+        <v>0.5839915943557298</v>
       </c>
       <c r="F32">
-        <v>0.16719219482007447</v>
+        <v>0.16202941265620183</v>
       </c>
       <c r="G32">
         <v>0.0</v>
@@ -4627,19 +4633,19 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>0.7500552219444306</v>
+        <v>0.7494956974834317</v>
       </c>
       <c r="C33">
-        <v>0.21222028675476956</v>
+        <v>0.2091409353067449</v>
       </c>
       <c r="D33">
         <v>0.0</v>
       </c>
       <c r="E33">
-        <v>0.600044177555544</v>
+        <v>0.5995965579867456</v>
       </c>
       <c r="F33">
-        <v>0.16977622940381573</v>
+        <v>0.16731274824539594</v>
       </c>
       <c r="G33">
         <v>0.0</v>
@@ -4650,19 +4656,19 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>0.7687941356109949</v>
+        <v>0.7795972265780089</v>
       </c>
       <c r="C34">
-        <v>0.2175647601333055</v>
+        <v>0.2233127486167252</v>
       </c>
       <c r="D34">
         <v>0.0</v>
       </c>
       <c r="E34">
-        <v>0.6150353084887963</v>
+        <v>0.6236777812624064</v>
       </c>
       <c r="F34">
-        <v>0.1740518081066444</v>
+        <v>0.17865019889338024</v>
       </c>
       <c r="G34">
         <v>0.0</v>
@@ -4730,7 +4736,7 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>67.50325913808854</v>
+        <v>67.49226369721264</v>
       </c>
       <c r="C6">
         <v>11.08916339999999</v>
@@ -4744,7 +4750,7 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>67.51212881179613</v>
+        <v>67.49941213335848</v>
       </c>
       <c r="C7">
         <v>11.08916339999999</v>
@@ -4758,7 +4764,7 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>67.51556247488553</v>
+        <v>67.50740341493277</v>
       </c>
       <c r="C8">
         <v>11.08916339999999</v>
@@ -4772,7 +4778,7 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>67.52476440804476</v>
+        <v>67.51499514783004</v>
       </c>
       <c r="C9">
         <v>11.08916339999999</v>
@@ -4786,7 +4792,7 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>67.4996382346052</v>
+        <v>67.49611445652734</v>
       </c>
       <c r="C10">
         <v>11.08916339999999</v>
@@ -4800,7 +4806,7 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>67.50271752530773</v>
+        <v>67.50163220345638</v>
       </c>
       <c r="C11">
         <v>11.08916339999999</v>
@@ -4814,13 +4820,13 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>67.50573533525785</v>
+        <v>67.50765855653763</v>
       </c>
       <c r="C12">
-        <v>11.08617357198996</v>
+        <v>11.08916339999999</v>
       </c>
       <c r="D12">
-        <v>4.016976644485251</v>
+        <v>4.017662550000014</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4828,13 +4834,13 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>67.51164700480726</v>
+        <v>67.51397742502192</v>
       </c>
       <c r="C13">
-        <v>11.085734182836761</v>
+        <v>11.08916339999999</v>
       </c>
       <c r="D13">
-        <v>4.0168623275184006</v>
+        <v>4.017662550000014</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4842,13 +4848,13 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>67.51589799145043</v>
+        <v>67.51981701154902</v>
       </c>
       <c r="C14">
-        <v>11.085384577240784</v>
+        <v>11.08916339999999</v>
       </c>
       <c r="D14">
-        <v>4.016835554529403</v>
+        <v>4.017662550000014</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4856,13 +4862,13 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>67.54172646623282</v>
+        <v>67.54308808702183</v>
       </c>
       <c r="C15">
-        <v>11.084710963907405</v>
+        <v>11.08916339999999</v>
       </c>
       <c r="D15">
-        <v>2.231813779793056</v>
+        <v>2.23203475</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4870,13 +4876,13 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>67.54894317080368</v>
+        <v>67.5563541343866</v>
       </c>
       <c r="C16">
-        <v>11.085386542192568</v>
+        <v>11.08916339999999</v>
       </c>
       <c r="D16">
-        <v>2.23203025</v>
+        <v>2.23203475</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4884,13 +4890,13 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>67.55619458914776</v>
+        <v>67.56810791708715</v>
       </c>
       <c r="C17">
-        <v>11.087761832312856</v>
+        <v>11.092760785674532</v>
       </c>
       <c r="D17">
-        <v>2.23203025</v>
+        <v>2.23203475</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4898,10 +4904,10 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>67.56410527775152</v>
+        <v>67.57489113080511</v>
       </c>
       <c r="C18">
-        <v>11.088646287463645</v>
+        <v>11.092760785674532</v>
       </c>
       <c r="D18">
         <v>2.23203475</v>
@@ -4912,10 +4918,10 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>67.57240168069578</v>
+        <v>67.43307690870782</v>
       </c>
       <c r="C19">
-        <v>11.088634486540096</v>
+        <v>11.09079664097786</v>
       </c>
       <c r="D19">
         <v>2.23203475</v>
@@ -4926,10 +4932,10 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>67.58683461711287</v>
+        <v>67.58731125862501</v>
       </c>
       <c r="C20">
-        <v>11.089051451279847</v>
+        <v>11.092760785674532</v>
       </c>
       <c r="D20">
         <v>0.0</v>
@@ -4940,10 +4946,10 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>67.59161542916655</v>
+        <v>67.59172117792117</v>
       </c>
       <c r="C21">
-        <v>11.08916339999999</v>
+        <v>11.092760785674532</v>
       </c>
       <c r="D21">
         <v>0.0</v>
@@ -4954,10 +4960,10 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>67.59441161821358</v>
+        <v>67.55616306700377</v>
       </c>
       <c r="C22">
-        <v>11.13974213272947</v>
+        <v>20.539627564055603</v>
       </c>
       <c r="D22">
         <v>0.0</v>
@@ -4968,10 +4974,10 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>67.59763264045196</v>
+        <v>67.56456515801108</v>
       </c>
       <c r="C23">
-        <v>11.13974213272947</v>
+        <v>20.539627564055603</v>
       </c>
       <c r="D23">
         <v>0.0</v>
@@ -4982,10 +4988,10 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>67.60002198749068</v>
+        <v>67.38529784422467</v>
       </c>
       <c r="C24">
-        <v>11.13974213272947</v>
+        <v>20.53258503094198</v>
       </c>
       <c r="D24">
         <v>0.0</v>
@@ -4996,10 +5002,10 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>59.49555939607247</v>
+        <v>59.48656762088007</v>
       </c>
       <c r="C25">
-        <v>11.13974213272947</v>
+        <v>20.539627564055603</v>
       </c>
       <c r="D25">
         <v>0.0</v>
@@ -5010,10 +5016,10 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>67.60172198665762</v>
+        <v>67.44298117590145</v>
       </c>
       <c r="C26">
-        <v>11.13974213272947</v>
+        <v>20.53909208190718</v>
       </c>
       <c r="D26">
         <v>0.0</v>
@@ -5024,10 +5030,10 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>67.556773334927</v>
+        <v>67.32026464735345</v>
       </c>
       <c r="C27">
-        <v>25.4813832471035</v>
+        <v>44.51751392769135</v>
       </c>
       <c r="D27">
         <v>0.0</v>
@@ -5038,10 +5044,10 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>67.56384945364717</v>
+        <v>67.36006722576269</v>
       </c>
       <c r="C28">
-        <v>25.4813832471035</v>
+        <v>44.5175464016096</v>
       </c>
       <c r="D28">
         <v>0.0</v>
@@ -5052,10 +5058,10 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>67.57053018868623</v>
+        <v>67.39200433337521</v>
       </c>
       <c r="C29">
-        <v>25.4813832471035</v>
+        <v>44.51757887552785</v>
       </c>
       <c r="D29">
         <v>0.0</v>
@@ -5066,10 +5072,10 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>59.48749637819917</v>
+        <v>59.41397656537126</v>
       </c>
       <c r="C30">
-        <v>25.4813832471035</v>
+        <v>44.51818441198558</v>
       </c>
       <c r="D30">
         <v>0.0</v>
@@ -5080,10 +5086,10 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>67.58151101297774</v>
+        <v>67.44560198012105</v>
       </c>
       <c r="C31">
-        <v>25.4813832471035</v>
+        <v>44.51818441198558</v>
       </c>
       <c r="D31">
         <v>0.0</v>
@@ -5094,10 +5100,10 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>67.51377089171943</v>
+        <v>66.72568449383552</v>
       </c>
       <c r="C32">
-        <v>38.05919469977984</v>
+        <v>69.63360003369185</v>
       </c>
       <c r="D32">
         <v>0.0</v>
@@ -5108,10 +5114,10 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>67.52791260049999</v>
+        <v>66.81989220335561</v>
       </c>
       <c r="C33">
-        <v>38.05919469977984</v>
+        <v>69.6341449498882</v>
       </c>
       <c r="D33">
         <v>0.0</v>
@@ -5122,10 +5128,10 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>67.53762768641812</v>
+        <v>66.00274969574203</v>
       </c>
       <c r="C34">
-        <v>38.05919469977984</v>
+        <v>69.59291716411563</v>
       </c>
       <c r="D34">
         <v>0.0</v>
@@ -5138,268 +5144,364 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>72.99328676579982</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>67.8072781992243</v>
+      </c>
+      <c r="C5">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>46.169524178143774</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>46.16948226057717</v>
+      </c>
+      <c r="C6">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>47.05971614077977</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>47.05957498891443</v>
+      </c>
+      <c r="C7">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>46.70994482289439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>46.798353984439196</v>
+      </c>
+      <c r="C8">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>47.56865520336712</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>47.66122266334186</v>
+      </c>
+      <c r="C9">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>18.97271613417021</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>18.1176211848974</v>
+      </c>
+      <c r="C10">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>19.54674119383585</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>18.679169257445775</v>
+      </c>
+      <c r="C11">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>20.128414657141015</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>19.24814911297695</v>
+      </c>
+      <c r="C12">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>20.718735284642204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>19.824868930054855</v>
+      </c>
+      <c r="C13">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>21.316128908853816</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>20.40910603391831</v>
+      </c>
+      <c r="C14">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>15.911233808367353</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>14.105803649362626</v>
+      </c>
+      <c r="C15">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>17.446975540498425</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>15.501199026887853</v>
+      </c>
+      <c r="C16">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>19.053256914007296</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>16.970498371111464</v>
+      </c>
+      <c r="C17">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>20.476482841842415</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>18.43699545855146</v>
+      </c>
+      <c r="C18">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>22.178962399728615</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>20.0</v>
+      </c>
+      <c r="C19">
+        <v>708.5741996233517</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>17.04837427467118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>16.53642336738266</v>
+      </c>
+      <c r="C20">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>18.471206102432618</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>17.93033926878534</v>
+      </c>
+      <c r="C21">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>19.85158312529389</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>17.716010310639025</v>
+      </c>
+      <c r="C22">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>20.992781566750278</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>18.636063789546405</v>
+      </c>
+      <c r="C23">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>22.523429697682296</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>20.0</v>
+      </c>
+      <c r="C24">
+        <v>708.5741996233525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>21.171313893801067</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>19.989786705809536</v>
+      </c>
+      <c r="C25">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>21.1485281043977</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>20.0</v>
+      </c>
+      <c r="C26">
+        <v>708.574199623352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>20.061528341221162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>17.643673760104623</v>
+      </c>
+      <c r="C27">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>21.18161354512578</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>18.611526045452997</v>
+      </c>
+      <c r="C28">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>22.5664475800926</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>19.859419064327017</v>
+      </c>
+      <c r="C29">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>22.576541420401774</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>19.913128032123492</v>
+      </c>
+      <c r="C30">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>22.57545875050855</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>19.980377020947138</v>
+      </c>
+      <c r="C31">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>21.87182142343567</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>17.92048603872539</v>
+      </c>
+      <c r="C32">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>22.994534238451642</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>18.952512288547883</v>
+      </c>
+      <c r="C33">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>24.328306356296142</v>
+        <v>20.0</v>
+      </c>
+      <c r="C34">
+        <v>7236.55251572327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change method=2 of subproblems
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -599,19 +599,19 @@
         <v>0.0</v>
       </c>
       <c r="C5">
-        <v>803.9610370387693</v>
+        <v>1276.773278358825</v>
       </c>
       <c r="D5">
         <v>0.0</v>
       </c>
       <c r="E5">
-        <v>1497.363716590231</v>
+        <v>986.8269011091952</v>
       </c>
       <c r="F5">
-        <v>2297.9611550761024</v>
+        <v>2116.15720057971</v>
       </c>
       <c r="G5">
-        <v>10000.0</v>
+        <v>9999.999999999998</v>
       </c>
       <c r="H5">
         <v>0.0</v>
@@ -620,7 +620,7 @@
         <v>0.0</v>
       </c>
       <c r="J5">
-        <v>0.0</v>
+        <v>4.6682172688630885</v>
       </c>
       <c r="K5">
         <v>19000.0</v>
@@ -632,10 +632,10 @@
         <v>0.0</v>
       </c>
       <c r="O5">
-        <v>430.8730349492289</v>
+        <v>429.84062962774675</v>
       </c>
       <c r="P5">
-        <v>87.47013812979615</v>
+        <v>87.84306536156468</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -810,7 +810,7 @@
         <v>0.0</v>
       </c>
       <c r="C10">
-        <v>5960.562454366782</v>
+        <v>6026.519272133795</v>
       </c>
       <c r="D10">
         <v>0.0</v>
@@ -1015,16 +1015,16 @@
         <v>0.0</v>
       </c>
       <c r="C15">
-        <v>5705.43579468594</v>
+        <v>5234.760016720449</v>
       </c>
       <c r="D15">
-        <v>0.1330347427099241</v>
+        <v>0.0</v>
       </c>
       <c r="E15">
-        <v>613.9063589030648</v>
+        <v>1165.5334766583694</v>
       </c>
       <c r="F15">
-        <v>118.97250952878312</v>
+        <v>777.2796703495719</v>
       </c>
       <c r="G15">
         <v>0.0</v>
@@ -1036,13 +1036,13 @@
         <v>0.0</v>
       </c>
       <c r="J15">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K15">
         <v>0.0</v>
       </c>
       <c r="L15">
-        <v>1.3300625785409543</v>
+        <v>632.7673767050928</v>
       </c>
       <c r="M15">
         <v>0.0</v>
@@ -1220,16 +1220,16 @@
         <v>0.0</v>
       </c>
       <c r="C20">
-        <v>3479.3746248175817</v>
+        <v>3911.087815060566</v>
       </c>
       <c r="D20">
-        <v>1038.9255100642702</v>
+        <v>529.0607494311558</v>
       </c>
       <c r="E20">
-        <v>4395.68207624171</v>
+        <v>5017.895662056333</v>
       </c>
       <c r="F20">
-        <v>1744.8476670371006</v>
+        <v>1092.2514932849176</v>
       </c>
       <c r="G20">
         <v>0.0</v>
@@ -1247,7 +1247,7 @@
         <v>0.0</v>
       </c>
       <c r="L20">
-        <v>3492.7931345445254</v>
+        <v>2822.368383872764</v>
       </c>
       <c r="M20">
         <v>0.0</v>
@@ -1422,19 +1422,19 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>127.98496165592496</v>
+        <v>0.0</v>
       </c>
       <c r="C25">
-        <v>3403.7662248724164</v>
+        <v>3402.675694264999</v>
       </c>
       <c r="D25">
-        <v>2461.268025575422</v>
+        <v>2432.321252961973</v>
       </c>
       <c r="E25">
-        <v>3188.614262169607</v>
+        <v>1618.7659998984818</v>
       </c>
       <c r="F25">
-        <v>1197.591562259594</v>
+        <v>1786.9058066937228</v>
       </c>
       <c r="G25">
         <v>0.0</v>
@@ -1452,7 +1452,7 @@
         <v>3000.0</v>
       </c>
       <c r="L25">
-        <v>8865.59964266673</v>
+        <v>8176.860596438973</v>
       </c>
       <c r="M25">
         <v>0.0</v>
@@ -1633,13 +1633,13 @@
         <v>0.0</v>
       </c>
       <c r="D30">
-        <v>1234.925228422304</v>
+        <v>0.0</v>
       </c>
       <c r="E30">
-        <v>940.3228063349052</v>
+        <v>2645.041468580279</v>
       </c>
       <c r="F30">
-        <v>3607.424493376394</v>
+        <v>1792.018518084984</v>
       </c>
       <c r="G30">
         <v>0.0</v>
@@ -1651,13 +1651,13 @@
         <v>0.0</v>
       </c>
       <c r="J30">
-        <v>0.0</v>
+        <v>152.1135156632712</v>
       </c>
       <c r="K30">
         <v>3000.0</v>
       </c>
       <c r="L30">
-        <v>9287.12563559234</v>
+        <v>9062.553729935538</v>
       </c>
       <c r="M30">
         <v>0.0</v>
@@ -1977,10 +1977,10 @@
         <v>5500.0</v>
       </c>
       <c r="O5">
-        <v>90.9513552166113</v>
+        <v>91.12853445632685</v>
       </c>
       <c r="P5">
-        <v>252.45154160282146</v>
+        <v>250.86902980985514</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2000,7 +2000,7 @@
         <v>17000.0</v>
       </c>
       <c r="F6">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G6">
         <v>5000.0</v>
@@ -2012,7 +2012,7 @@
         <v>1000.0</v>
       </c>
       <c r="J6">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K6">
         <v>25000.0</v>
@@ -2041,7 +2041,7 @@
         <v>17000.0</v>
       </c>
       <c r="F7">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G7">
         <v>5000.0</v>
@@ -2053,7 +2053,7 @@
         <v>1000.0</v>
       </c>
       <c r="J7">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K7">
         <v>25000.0</v>
@@ -2079,10 +2079,10 @@
         <v>5000.0</v>
       </c>
       <c r="E8">
-        <v>18497.363716590233</v>
+        <v>17986.826901109194</v>
       </c>
       <c r="F8">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G8">
         <v>5000.0</v>
@@ -2094,7 +2094,7 @@
         <v>1000.0</v>
       </c>
       <c r="J8">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K8">
         <v>25000.0</v>
@@ -2120,10 +2120,10 @@
         <v>5000.0</v>
       </c>
       <c r="E9">
-        <v>18497.363716590233</v>
+        <v>17986.826901109194</v>
       </c>
       <c r="F9">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G9">
         <v>5000.0</v>
@@ -2135,7 +2135,7 @@
         <v>1000.0</v>
       </c>
       <c r="J9">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K9">
         <v>25000.0</v>
@@ -2155,19 +2155,19 @@
         <v>10000.0</v>
       </c>
       <c r="C10">
-        <v>2803.961037038769</v>
+        <v>3276.7732783588253</v>
       </c>
       <c r="D10">
         <v>4000.0</v>
       </c>
       <c r="E10">
-        <v>17497.363716590233</v>
+        <v>16986.826901109194</v>
       </c>
       <c r="F10">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G10">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H10">
         <v>2000.0</v>
@@ -2176,7 +2176,7 @@
         <v>1000.0</v>
       </c>
       <c r="J10">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K10">
         <v>25000.0</v>
@@ -2196,19 +2196,19 @@
         <v>10000.0</v>
       </c>
       <c r="C11">
-        <v>2803.961037038769</v>
+        <v>3276.7732783588253</v>
       </c>
       <c r="D11">
         <v>4000.0</v>
       </c>
       <c r="E11">
-        <v>17497.363716590233</v>
+        <v>16986.826901109194</v>
       </c>
       <c r="F11">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G11">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H11">
         <v>2000.0</v>
@@ -2217,7 +2217,7 @@
         <v>1000.0</v>
       </c>
       <c r="J11">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K11">
         <v>25000.0</v>
@@ -2237,19 +2237,19 @@
         <v>10000.0</v>
       </c>
       <c r="C12">
-        <v>2803.961037038769</v>
+        <v>3276.7732783588253</v>
       </c>
       <c r="D12">
         <v>4000.0</v>
       </c>
       <c r="E12">
-        <v>17497.363716590233</v>
+        <v>16986.826901109194</v>
       </c>
       <c r="F12">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G12">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H12">
         <v>2000.0</v>
@@ -2258,7 +2258,7 @@
         <v>1000.0</v>
       </c>
       <c r="J12">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K12">
         <v>25000.0</v>
@@ -2278,19 +2278,19 @@
         <v>10000.0</v>
       </c>
       <c r="C13">
-        <v>2803.961037038769</v>
+        <v>3276.7732783588253</v>
       </c>
       <c r="D13">
         <v>4000.0</v>
       </c>
       <c r="E13">
-        <v>17497.363716590233</v>
+        <v>16986.826901109194</v>
       </c>
       <c r="F13">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G13">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H13">
         <v>2000.0</v>
@@ -2299,7 +2299,7 @@
         <v>1000.0</v>
       </c>
       <c r="J13">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K13">
         <v>25000.0</v>
@@ -2319,19 +2319,19 @@
         <v>10000.0</v>
       </c>
       <c r="C14">
-        <v>2803.961037038769</v>
+        <v>3276.7732783588253</v>
       </c>
       <c r="D14">
         <v>4000.0</v>
       </c>
       <c r="E14">
-        <v>17497.363716590233</v>
+        <v>16986.826901109194</v>
       </c>
       <c r="F14">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G14">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H14">
         <v>2000.0</v>
@@ -2340,7 +2340,7 @@
         <v>1000.0</v>
       </c>
       <c r="J14">
-        <v>500.0</v>
+        <v>504.6682172688631</v>
       </c>
       <c r="K14">
         <v>25000.0</v>
@@ -2360,19 +2360,19 @@
         <v>8000.0</v>
       </c>
       <c r="C15">
-        <v>8764.52349140555</v>
+        <v>9303.29255049262</v>
       </c>
       <c r="D15">
         <v>3500.0</v>
       </c>
       <c r="E15">
-        <v>15497.363716590231</v>
+        <v>14986.826901109194</v>
       </c>
       <c r="F15">
-        <v>3297.9611550761024</v>
+        <v>3116.15720057971</v>
       </c>
       <c r="G15">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H15">
         <v>2000.0</v>
@@ -2381,7 +2381,7 @@
         <v>1000.0</v>
       </c>
       <c r="J15">
-        <v>0.0</v>
+        <v>4.6682172688630885</v>
       </c>
       <c r="K15">
         <v>25000.0</v>
@@ -2401,19 +2401,19 @@
         <v>8000.0</v>
       </c>
       <c r="C16">
-        <v>8764.52349140555</v>
+        <v>9303.29255049262</v>
       </c>
       <c r="D16">
         <v>3500.0</v>
       </c>
       <c r="E16">
-        <v>15497.363716590231</v>
+        <v>14986.826901109194</v>
       </c>
       <c r="F16">
-        <v>3416.9336646048855</v>
+        <v>3893.436870929282</v>
       </c>
       <c r="G16">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H16">
         <v>2000.0</v>
@@ -2422,7 +2422,7 @@
         <v>1000.0</v>
       </c>
       <c r="J16">
-        <v>0.0</v>
+        <v>21.229268571016505</v>
       </c>
       <c r="K16">
         <v>25000.0</v>
@@ -2442,19 +2442,19 @@
         <v>8000.0</v>
       </c>
       <c r="C17">
-        <v>8764.52349140555</v>
+        <v>9303.29255049262</v>
       </c>
       <c r="D17">
-        <v>3500.13303474271</v>
+        <v>3500.0</v>
       </c>
       <c r="E17">
-        <v>15497.363716590231</v>
+        <v>14986.826901109194</v>
       </c>
       <c r="F17">
-        <v>3416.9336646048855</v>
+        <v>3893.436870929282</v>
       </c>
       <c r="G17">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H17">
         <v>2000.0</v>
@@ -2463,13 +2463,13 @@
         <v>1000.0</v>
       </c>
       <c r="J17">
-        <v>0.0</v>
+        <v>21.229268571016505</v>
       </c>
       <c r="K17">
         <v>25000.0</v>
       </c>
       <c r="L17">
-        <v>4101.330062578541</v>
+        <v>4732.767376705093</v>
       </c>
       <c r="M17">
         <v>2500.0</v>
@@ -2483,19 +2483,19 @@
         <v>8000.0</v>
       </c>
       <c r="C18">
-        <v>8764.52349140555</v>
+        <v>9303.29255049262</v>
       </c>
       <c r="D18">
-        <v>3500.13303474271</v>
+        <v>3500.0</v>
       </c>
       <c r="E18">
-        <v>16111.270075493296</v>
+        <v>16152.360377767563</v>
       </c>
       <c r="F18">
-        <v>3416.9336646048855</v>
+        <v>3893.436870929282</v>
       </c>
       <c r="G18">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H18">
         <v>2000.0</v>
@@ -2504,13 +2504,13 @@
         <v>1000.0</v>
       </c>
       <c r="J18">
-        <v>0.0</v>
+        <v>21.229268571016505</v>
       </c>
       <c r="K18">
         <v>25000.0</v>
       </c>
       <c r="L18">
-        <v>4101.330062578541</v>
+        <v>4732.767376705093</v>
       </c>
       <c r="M18">
         <v>2500.0</v>
@@ -2524,19 +2524,19 @@
         <v>8000.0</v>
       </c>
       <c r="C19">
-        <v>8764.52349140555</v>
+        <v>9303.29255049262</v>
       </c>
       <c r="D19">
-        <v>3500.13303474271</v>
+        <v>3500.0</v>
       </c>
       <c r="E19">
-        <v>16111.270075493296</v>
+        <v>16152.360377767563</v>
       </c>
       <c r="F19">
-        <v>3416.9336646048855</v>
+        <v>3893.436870929282</v>
       </c>
       <c r="G19">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H19">
         <v>2000.0</v>
@@ -2545,13 +2545,13 @@
         <v>1000.0</v>
       </c>
       <c r="J19">
-        <v>0.0</v>
+        <v>21.229268571016505</v>
       </c>
       <c r="K19">
         <v>25000.0</v>
       </c>
       <c r="L19">
-        <v>4101.330062578541</v>
+        <v>4732.767376705093</v>
       </c>
       <c r="M19">
         <v>2500.0</v>
@@ -2565,19 +2565,19 @@
         <v>6000.0</v>
       </c>
       <c r="C20">
-        <v>14469.95928609149</v>
+        <v>14538.05256721307</v>
       </c>
       <c r="D20">
-        <v>2500.13303474271</v>
+        <v>2500.0</v>
       </c>
       <c r="E20">
-        <v>12111.270075493296</v>
+        <v>12152.360377767563</v>
       </c>
       <c r="F20">
-        <v>2416.9336646048855</v>
+        <v>2893.436870929282</v>
       </c>
       <c r="G20">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H20">
         <v>2000.0</v>
@@ -2586,13 +2586,13 @@
         <v>1000.0</v>
       </c>
       <c r="J20">
-        <v>0.0</v>
+        <v>21.229268571016505</v>
       </c>
       <c r="K20">
         <v>25000.0</v>
       </c>
       <c r="L20">
-        <v>4101.330062578541</v>
+        <v>4732.767376705093</v>
       </c>
       <c r="M20">
         <v>0.0</v>
@@ -2606,19 +2606,19 @@
         <v>6000.0</v>
       </c>
       <c r="C21">
-        <v>14469.95928609149</v>
+        <v>14538.05256721307</v>
       </c>
       <c r="D21">
-        <v>2500.13303474271</v>
+        <v>2500.0</v>
       </c>
       <c r="E21">
-        <v>12111.270075493296</v>
+        <v>12152.360377767563</v>
       </c>
       <c r="F21">
-        <v>4161.781331641986</v>
+        <v>3985.6883642141997</v>
       </c>
       <c r="G21">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H21">
         <v>2000.0</v>
@@ -2627,13 +2627,13 @@
         <v>1000.0</v>
       </c>
       <c r="J21">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K21">
         <v>25000.0</v>
       </c>
       <c r="L21">
-        <v>4101.330062578541</v>
+        <v>4732.767376705093</v>
       </c>
       <c r="M21">
         <v>0.0</v>
@@ -2647,19 +2647,19 @@
         <v>6000.0</v>
       </c>
       <c r="C22">
-        <v>14469.95928609149</v>
+        <v>14538.05256721307</v>
       </c>
       <c r="D22">
-        <v>3539.0585448069805</v>
+        <v>3029.0607494311557</v>
       </c>
       <c r="E22">
-        <v>12111.270075493296</v>
+        <v>12152.360377767563</v>
       </c>
       <c r="F22">
-        <v>4161.781331641986</v>
+        <v>3985.6883642141997</v>
       </c>
       <c r="G22">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H22">
         <v>2000.0</v>
@@ -2668,13 +2668,13 @@
         <v>1000.0</v>
       </c>
       <c r="J22">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K22">
         <v>25000.0</v>
       </c>
       <c r="L22">
-        <v>7594.123197123066</v>
+        <v>7555.135760577857</v>
       </c>
       <c r="M22">
         <v>0.0</v>
@@ -2688,19 +2688,19 @@
         <v>6000.0</v>
       </c>
       <c r="C23">
-        <v>14469.95928609149</v>
+        <v>14538.05256721307</v>
       </c>
       <c r="D23">
-        <v>3539.0585448069805</v>
+        <v>3029.0607494311557</v>
       </c>
       <c r="E23">
-        <v>16506.952151735008</v>
+        <v>17170.256039823897</v>
       </c>
       <c r="F23">
-        <v>4161.781331641986</v>
+        <v>3985.6883642141997</v>
       </c>
       <c r="G23">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H23">
         <v>2000.0</v>
@@ -2709,13 +2709,13 @@
         <v>1000.0</v>
       </c>
       <c r="J23">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K23">
         <v>25000.0</v>
       </c>
       <c r="L23">
-        <v>7594.123197123066</v>
+        <v>7555.135760577857</v>
       </c>
       <c r="M23">
         <v>0.0</v>
@@ -2729,19 +2729,19 @@
         <v>6000.0</v>
       </c>
       <c r="C24">
-        <v>14469.95928609149</v>
+        <v>14538.05256721307</v>
       </c>
       <c r="D24">
-        <v>3539.0585448069805</v>
+        <v>3029.0607494311557</v>
       </c>
       <c r="E24">
-        <v>16506.952151735008</v>
+        <v>17170.256039823897</v>
       </c>
       <c r="F24">
-        <v>4161.781331641986</v>
+        <v>3985.6883642141997</v>
       </c>
       <c r="G24">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H24">
         <v>2000.0</v>
@@ -2750,13 +2750,13 @@
         <v>1000.0</v>
       </c>
       <c r="J24">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K24">
         <v>25000.0</v>
       </c>
       <c r="L24">
-        <v>7594.123197123066</v>
+        <v>7555.135760577857</v>
       </c>
       <c r="M24">
         <v>0.0</v>
@@ -2770,19 +2770,19 @@
         <v>5000.0</v>
       </c>
       <c r="C25">
-        <v>17949.333910909074</v>
+        <v>18449.140382273636</v>
       </c>
       <c r="D25">
-        <v>2039.05854480698</v>
+        <v>1529.0607494311557</v>
       </c>
       <c r="E25">
-        <v>13506.952151735006</v>
+        <v>14170.256039823897</v>
       </c>
       <c r="F25">
-        <v>4161.781331641986</v>
+        <v>3985.6883642141997</v>
       </c>
       <c r="G25">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H25">
         <v>2000.0</v>
@@ -2791,13 +2791,13 @@
         <v>1000.0</v>
       </c>
       <c r="J25">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K25">
         <v>22000.0</v>
       </c>
       <c r="L25">
-        <v>7594.123197123066</v>
+        <v>7555.135760577857</v>
       </c>
       <c r="M25">
         <v>0.0</v>
@@ -2811,19 +2811,19 @@
         <v>5000.0</v>
       </c>
       <c r="C26">
-        <v>17949.333910909074</v>
+        <v>18449.140382273636</v>
       </c>
       <c r="D26">
-        <v>2039.05854480698</v>
+        <v>1529.0607494311557</v>
       </c>
       <c r="E26">
-        <v>13506.952151735006</v>
+        <v>14170.256039823897</v>
       </c>
       <c r="F26">
-        <v>5359.37289390158</v>
+        <v>5772.5941709079225</v>
       </c>
       <c r="G26">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H26">
         <v>2000.0</v>
@@ -2832,13 +2832,13 @@
         <v>1000.0</v>
       </c>
       <c r="J26">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K26">
         <v>25000.0</v>
       </c>
       <c r="L26">
-        <v>7594.123197123066</v>
+        <v>7555.135760577857</v>
       </c>
       <c r="M26">
         <v>0.0</v>
@@ -2852,19 +2852,19 @@
         <v>5000.0</v>
       </c>
       <c r="C27">
-        <v>17949.333910909074</v>
+        <v>18449.140382273636</v>
       </c>
       <c r="D27">
-        <v>4500.326570382402</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E27">
-        <v>13506.952151735006</v>
+        <v>14170.256039823897</v>
       </c>
       <c r="F27">
-        <v>5359.37289390158</v>
+        <v>5772.5941709079225</v>
       </c>
       <c r="G27">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H27">
         <v>2000.0</v>
@@ -2873,13 +2873,13 @@
         <v>1000.0</v>
       </c>
       <c r="J27">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K27">
         <v>25000.0</v>
       </c>
       <c r="L27">
-        <v>16459.722839789796</v>
+        <v>15731.99635701683</v>
       </c>
       <c r="M27">
         <v>0.0</v>
@@ -2893,19 +2893,19 @@
         <v>5000.0</v>
       </c>
       <c r="C28">
-        <v>17949.333910909074</v>
+        <v>18449.140382273636</v>
       </c>
       <c r="D28">
-        <v>4500.326570382402</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E28">
-        <v>16695.566413904613</v>
+        <v>15789.022039722378</v>
       </c>
       <c r="F28">
-        <v>5359.37289390158</v>
+        <v>5772.5941709079225</v>
       </c>
       <c r="G28">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H28">
         <v>2000.0</v>
@@ -2914,13 +2914,13 @@
         <v>1000.0</v>
       </c>
       <c r="J28">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K28">
         <v>25000.0</v>
       </c>
       <c r="L28">
-        <v>16459.722839789796</v>
+        <v>15731.99635701683</v>
       </c>
       <c r="M28">
         <v>0.0</v>
@@ -2934,19 +2934,19 @@
         <v>5000.0</v>
       </c>
       <c r="C29">
-        <v>17949.333910909074</v>
+        <v>18449.140382273636</v>
       </c>
       <c r="D29">
-        <v>4500.326570382402</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E29">
-        <v>16695.566413904613</v>
+        <v>15789.022039722378</v>
       </c>
       <c r="F29">
-        <v>5359.37289390158</v>
+        <v>5772.5941709079225</v>
       </c>
       <c r="G29">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H29">
         <v>2000.0</v>
@@ -2955,13 +2955,13 @@
         <v>1000.0</v>
       </c>
       <c r="J29">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K29">
         <v>25000.0</v>
       </c>
       <c r="L29">
-        <v>16459.722839789796</v>
+        <v>15731.99635701683</v>
       </c>
       <c r="M29">
         <v>0.0</v>
@@ -2972,22 +2972,22 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>4127.984961655925</v>
+        <v>4000.0</v>
       </c>
       <c r="C30">
-        <v>21353.10013578149</v>
+        <v>21851.816076538635</v>
       </c>
       <c r="D30">
-        <v>4500.326570382402</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E30">
-        <v>14695.566413904613</v>
+        <v>13789.022039722378</v>
       </c>
       <c r="F30">
-        <v>5359.37289390158</v>
+        <v>5772.5941709079225</v>
       </c>
       <c r="G30">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H30">
         <v>2000.0</v>
@@ -2996,13 +2996,13 @@
         <v>1000.0</v>
       </c>
       <c r="J30">
-        <v>0.0</v>
+        <v>16.561051302153416</v>
       </c>
       <c r="K30">
         <v>22000.0</v>
       </c>
       <c r="L30">
-        <v>16459.722839789796</v>
+        <v>15731.99635701683</v>
       </c>
       <c r="M30">
         <v>0.0</v>
@@ -3013,22 +3013,22 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>4127.984961655925</v>
+        <v>4000.0</v>
       </c>
       <c r="C31">
-        <v>21353.10013578149</v>
+        <v>21851.816076538635</v>
       </c>
       <c r="D31">
-        <v>4500.326570382402</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E31">
-        <v>14695.566413904613</v>
+        <v>13789.022039722378</v>
       </c>
       <c r="F31">
-        <v>6668.836232201871</v>
+        <v>5448.455488413196</v>
       </c>
       <c r="G31">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H31">
         <v>2000.0</v>
@@ -3037,13 +3037,13 @@
         <v>1000.0</v>
       </c>
       <c r="J31">
-        <v>0.0</v>
+        <v>152.1135156632712</v>
       </c>
       <c r="K31">
         <v>25000.0</v>
       </c>
       <c r="L31">
-        <v>16459.722839789796</v>
+        <v>15731.99635701683</v>
       </c>
       <c r="M31">
         <v>0.0</v>
@@ -3054,22 +3054,22 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>4127.984961655925</v>
+        <v>4000.0</v>
       </c>
       <c r="C32">
-        <v>21353.10013578149</v>
+        <v>21851.816076538635</v>
       </c>
       <c r="D32">
-        <v>5735.251798804706</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E32">
-        <v>14695.566413904613</v>
+        <v>13789.022039722378</v>
       </c>
       <c r="F32">
-        <v>6668.836232201871</v>
+        <v>5448.455488413196</v>
       </c>
       <c r="G32">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H32">
         <v>2000.0</v>
@@ -3078,13 +3078,13 @@
         <v>1000.0</v>
       </c>
       <c r="J32">
-        <v>0.0</v>
+        <v>152.1135156632712</v>
       </c>
       <c r="K32">
         <v>25000.0</v>
       </c>
       <c r="L32">
-        <v>25746.848475382136</v>
+        <v>24794.550086952368</v>
       </c>
       <c r="M32">
         <v>0.0</v>
@@ -3095,22 +3095,22 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>4127.984961655925</v>
+        <v>4000.0</v>
       </c>
       <c r="C33">
-        <v>21353.10013578149</v>
+        <v>21851.816076538635</v>
       </c>
       <c r="D33">
-        <v>5735.251798804706</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E33">
-        <v>15635.889220239518</v>
+        <v>16434.063508302657</v>
       </c>
       <c r="F33">
-        <v>6668.836232201871</v>
+        <v>5448.455488413196</v>
       </c>
       <c r="G33">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H33">
         <v>2000.0</v>
@@ -3119,13 +3119,13 @@
         <v>1000.0</v>
       </c>
       <c r="J33">
-        <v>0.0</v>
+        <v>152.1135156632712</v>
       </c>
       <c r="K33">
         <v>25000.0</v>
       </c>
       <c r="L33">
-        <v>25746.848475382136</v>
+        <v>24794.550086952368</v>
       </c>
       <c r="M33">
         <v>0.0</v>
@@ -3136,22 +3136,22 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>4127.984961655925</v>
+        <v>4000.0</v>
       </c>
       <c r="C34">
-        <v>21353.10013578149</v>
+        <v>21851.816076538635</v>
       </c>
       <c r="D34">
-        <v>5735.251798804706</v>
+        <v>3961.382002393129</v>
       </c>
       <c r="E34">
-        <v>15635.889220239518</v>
+        <v>16434.063508302657</v>
       </c>
       <c r="F34">
-        <v>6668.836232201871</v>
+        <v>5448.455488413196</v>
       </c>
       <c r="G34">
-        <v>15000.0</v>
+        <v>14999.999999999998</v>
       </c>
       <c r="H34">
         <v>2000.0</v>
@@ -3160,13 +3160,13 @@
         <v>1000.0</v>
       </c>
       <c r="J34">
-        <v>0.0</v>
+        <v>152.1135156632712</v>
       </c>
       <c r="K34">
         <v>25000.0</v>
       </c>
       <c r="L34">
-        <v>25746.848475382136</v>
+        <v>24794.550086952368</v>
       </c>
       <c r="M34">
         <v>0.0</v>
@@ -3238,16 +3238,16 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>11.492883591785887</v>
+        <v>11.492883591785874</v>
       </c>
       <c r="C5">
         <v>17.52</v>
       </c>
       <c r="D5">
-        <v>19.554394315687563</v>
+        <v>19.554394315687546</v>
       </c>
       <c r="E5">
-        <v>135.291997947918</v>
+        <v>135.29199794791808</v>
       </c>
       <c r="F5">
         <v>0.16042972465095315</v>
@@ -3261,22 +3261,22 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>4.466684303599806</v>
+        <v>4.466106990447277</v>
       </c>
       <c r="C6">
-        <v>16.93627944966481</v>
+        <v>16.936400041586825</v>
       </c>
       <c r="D6">
-        <v>9.118101501871484</v>
+        <v>9.117407803973459</v>
       </c>
       <c r="E6">
-        <v>104.8681725408936</v>
+        <v>104.86927626130385</v>
       </c>
       <c r="F6">
-        <v>0.08569427441655028</v>
+        <v>0.08382499059723801</v>
       </c>
       <c r="G6">
-        <v>43.213410482922974</v>
+        <v>43.21349471788488</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3284,22 +3284,22 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>4.773043142570225</v>
+        <v>4.7724537593585135</v>
       </c>
       <c r="C7">
-        <v>16.965512606351798</v>
+        <v>16.965611519786737</v>
       </c>
       <c r="D7">
-        <v>9.563565943270225</v>
+        <v>9.562872905496537</v>
       </c>
       <c r="E7">
-        <v>106.02458186400393</v>
+        <v>106.02571901128606</v>
       </c>
       <c r="F7">
-        <v>0.10154924242941013</v>
+        <v>0.09931624458549594</v>
       </c>
       <c r="G7">
-        <v>43.25139344695766</v>
+        <v>43.25151102108378</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3307,22 +3307,22 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>3.6091104630643396</v>
+        <v>4.075740362039916</v>
       </c>
       <c r="C8">
-        <v>16.99413825295042</v>
+        <v>16.99422561275059</v>
       </c>
       <c r="D8">
-        <v>7.575360306197158</v>
+        <v>8.339346106246326</v>
       </c>
       <c r="E8">
-        <v>111.14657040704283</v>
+        <v>109.90088657645084</v>
       </c>
       <c r="F8">
-        <v>0.05196259375661242</v>
+        <v>0.07140635125843159</v>
       </c>
       <c r="G8">
-        <v>43.28396537132581</v>
+        <v>43.28408484034222</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3330,22 +3330,22 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>3.876107114241729</v>
+        <v>4.363148296866731</v>
       </c>
       <c r="C9">
-        <v>17.020722131937312</v>
+        <v>17.02080411882238</v>
       </c>
       <c r="D9">
-        <v>7.955245815480021</v>
+        <v>8.749535533080216</v>
       </c>
       <c r="E9">
-        <v>112.42186728433019</v>
+        <v>111.12333134325439</v>
       </c>
       <c r="F9">
-        <v>0.06575920517584274</v>
+        <v>0.085654305504527</v>
       </c>
       <c r="G9">
-        <v>43.31528588228263</v>
+        <v>43.31539732196525</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3353,22 +3353,22 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>0.2940447868105326</v>
+        <v>0.29899811261164294</v>
       </c>
       <c r="C10">
-        <v>18.507707231488595</v>
+        <v>21.31446039125581</v>
       </c>
       <c r="D10">
-        <v>0.9028431216665117</v>
+        <v>0.9112990080968507</v>
       </c>
       <c r="E10">
-        <v>44.78879543618919</v>
+        <v>41.97953609905546</v>
       </c>
       <c r="F10">
         <v>0.0</v>
       </c>
       <c r="G10">
-        <v>123.08810613967549</v>
+        <v>123.08099814616193</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3376,22 +3376,22 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>0.3408855177021206</v>
+        <v>0.3462168634573464</v>
       </c>
       <c r="C11">
-        <v>18.703905840146255</v>
+        <v>21.546294293515672</v>
       </c>
       <c r="D11">
-        <v>0.9768771413804677</v>
+        <v>0.9859867794921783</v>
       </c>
       <c r="E11">
-        <v>46.1435047138381</v>
+        <v>43.294469171688</v>
       </c>
       <c r="F11">
         <v>0.0</v>
       </c>
       <c r="G11">
-        <v>123.40859733185158</v>
+        <v>123.40471993682388</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3399,22 +3399,22 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>0.39152666213244414</v>
+        <v>0.39737613087249357</v>
       </c>
       <c r="C12">
-        <v>18.897014999683062</v>
+        <v>21.77383249062819</v>
       </c>
       <c r="D12">
-        <v>1.054937855012834</v>
+        <v>1.0642541590562082</v>
       </c>
       <c r="E12">
-        <v>47.505838050719596</v>
+        <v>44.61940049485096</v>
       </c>
       <c r="F12">
         <v>0.0</v>
       </c>
       <c r="G12">
-        <v>123.71627959750774</v>
+        <v>123.71440401064314</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3422,22 +3422,22 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>0.44749591137700834</v>
+        <v>0.45386316448370717</v>
       </c>
       <c r="C13">
-        <v>19.091363557008886</v>
+        <v>21.999742784631845</v>
       </c>
       <c r="D13">
-        <v>1.133210897698477</v>
+        <v>1.1431558509505126</v>
       </c>
       <c r="E13">
-        <v>48.877377742168996</v>
+        <v>45.95502664811031</v>
       </c>
       <c r="F13">
         <v>0.0</v>
       </c>
       <c r="G13">
-        <v>124.00897401924342</v>
+        <v>124.0094193397102</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3445,22 +3445,22 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>0.506219216620154</v>
+        <v>0.5129137777622004</v>
       </c>
       <c r="C14">
-        <v>19.27818156869697</v>
+        <v>22.22085978211362</v>
       </c>
       <c r="D14">
-        <v>1.2183007505103933</v>
+        <v>1.2288532290210372</v>
       </c>
       <c r="E14">
-        <v>50.25655131062698</v>
+        <v>47.29753712297836</v>
       </c>
       <c r="F14">
         <v>0.0</v>
       </c>
       <c r="G14">
-        <v>124.29190629668412</v>
+        <v>124.29355030802678</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3468,22 +3468,22 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>0.12565968293048718</v>
+        <v>0.12364350214954554</v>
       </c>
       <c r="C15">
-        <v>50.81425523761625</v>
+        <v>52.89477917584495</v>
       </c>
       <c r="D15">
-        <v>0.47292002532360317</v>
+        <v>0.46931541434109225</v>
       </c>
       <c r="E15">
-        <v>23.283198698344158</v>
+        <v>21.206668250792887</v>
       </c>
       <c r="F15">
         <v>0.0</v>
       </c>
       <c r="G15">
-        <v>124.65998846716757</v>
+        <v>124.66106143969147</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3491,22 +3491,22 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>0.2199326624499516</v>
+        <v>0.21640351702295743</v>
       </c>
       <c r="C16">
-        <v>52.822172550077525</v>
+        <v>55.06088306301186</v>
       </c>
       <c r="D16">
-        <v>0.5993594581927059</v>
+        <v>0.5948430396031061</v>
       </c>
       <c r="E16">
-        <v>26.280665311932434</v>
+        <v>24.04756200956607</v>
       </c>
       <c r="F16">
         <v>0.0</v>
       </c>
       <c r="G16">
-        <v>125.41970654069635</v>
+        <v>125.42296886650541</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3514,22 +3514,22 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>0.34779517554800077</v>
+        <v>0.33202346566627955</v>
       </c>
       <c r="C17">
-        <v>54.713878893938094</v>
+        <v>56.44070019758514</v>
       </c>
       <c r="D17">
-        <v>0.7646360894632591</v>
+        <v>0.7390169120729226</v>
       </c>
       <c r="E17">
-        <v>29.39258740252358</v>
+        <v>26.440471934501574</v>
       </c>
       <c r="F17">
-        <v>0.0008497639380650798</v>
+        <v>0.0007784439694963948</v>
       </c>
       <c r="G17">
-        <v>126.10464244327521</v>
+        <v>125.67791498685523</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3537,22 +3537,22 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>0.4071133473143775</v>
+        <v>0.31149718785356806</v>
       </c>
       <c r="C18">
-        <v>56.491424925096574</v>
+        <v>58.377725408814804</v>
       </c>
       <c r="D18">
-        <v>0.8289308088779457</v>
+        <v>0.7012481775260258</v>
       </c>
       <c r="E18">
-        <v>32.85164314738478</v>
+        <v>29.891236994561012</v>
       </c>
       <c r="F18">
-        <v>0.0014374478900305622</v>
+        <v>0.000715356191486906</v>
       </c>
       <c r="G18">
-        <v>126.73260518048882</v>
+        <v>126.33478662545488</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3560,22 +3560,22 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>0.3707287097746543</v>
+        <v>0.46073522872875944</v>
       </c>
       <c r="C19">
-        <v>58.05228653175078</v>
+        <v>60.20347602081325</v>
       </c>
       <c r="D19">
-        <v>1.0349432274328414</v>
+        <v>0.8786838047524338</v>
       </c>
       <c r="E19">
-        <v>36.2361280592374</v>
+        <v>33.13095276280712</v>
       </c>
       <c r="F19">
-        <v>0.20804382571002197</v>
+        <v>0.002777548617055472</v>
       </c>
       <c r="G19">
-        <v>127.55104333805646</v>
+        <v>126.9295152789113</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3583,22 +3583,22 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>0.6150572816597963</v>
+        <v>0.5798791423917158</v>
       </c>
       <c r="C20">
-        <v>84.86597384657841</v>
+        <v>84.1441657951427</v>
       </c>
       <c r="D20">
-        <v>0.7077033559464845</v>
+        <v>0.6675111698746095</v>
       </c>
       <c r="E20">
-        <v>17.41274450457653</v>
+        <v>16.833676577492348</v>
       </c>
       <c r="F20">
-        <v>0.03175114172071534</v>
+        <v>0.03115051550990562</v>
       </c>
       <c r="G20">
-        <v>127.88594847825674</v>
+        <v>127.56376836678325</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3606,22 +3606,22 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>0.8074404428721602</v>
+        <v>0.762675510748826</v>
       </c>
       <c r="C21">
-        <v>87.69462949171029</v>
+        <v>87.01676603737512</v>
       </c>
       <c r="D21">
-        <v>0.875628838708774</v>
+        <v>0.8342026301961862</v>
       </c>
       <c r="E21">
-        <v>19.75454141474421</v>
+        <v>19.11873564315627</v>
       </c>
       <c r="F21">
-        <v>0.06872614094560778</v>
+        <v>0.06112398574813551</v>
       </c>
       <c r="G21">
-        <v>128.31918442008234</v>
+        <v>128.02384446690687</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3629,22 +3629,22 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>0.6931861358509351</v>
+        <v>0.7665954120562387</v>
       </c>
       <c r="C22">
-        <v>85.45472677200397</v>
+        <v>85.74565940359369</v>
       </c>
       <c r="D22">
-        <v>1.1814940533187872</v>
+        <v>1.0430772684458223</v>
       </c>
       <c r="E22">
-        <v>19.716366851267665</v>
+        <v>19.554381081634805</v>
       </c>
       <c r="F22">
-        <v>0.05469378453261846</v>
+        <v>0.06919523455209776</v>
       </c>
       <c r="G22">
-        <v>127.01091595292955</v>
+        <v>127.03519530517656</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3652,22 +3652,22 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>0.2184382022454988</v>
+        <v>0.1975466576080577</v>
       </c>
       <c r="C23">
-        <v>88.11219246650508</v>
+        <v>88.41972034441675</v>
       </c>
       <c r="D23">
-        <v>0.5520130053113396</v>
+        <v>0.42868503700328753</v>
       </c>
       <c r="E23">
-        <v>23.713716950925434</v>
+        <v>23.633255682217875</v>
       </c>
       <c r="F23">
-        <v>0.005521805235611288</v>
+        <v>0.004399384838179359</v>
       </c>
       <c r="G23">
-        <v>127.50235328685618</v>
+        <v>127.52488605854613</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3675,22 +3675,22 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>0.05527045329263642</v>
+        <v>0.304038707972448</v>
       </c>
       <c r="C24">
-        <v>90.51216704854355</v>
+        <v>90.96270176567688</v>
       </c>
       <c r="D24">
-        <v>0.6763092347771626</v>
+        <v>0.5198690690587717</v>
       </c>
       <c r="E24">
-        <v>26.49392393780331</v>
+        <v>26.441430627134284</v>
       </c>
       <c r="F24">
-        <v>0.2896965955153706</v>
+        <v>0.01197558056239286</v>
       </c>
       <c r="G24">
-        <v>128.2668534024937</v>
+        <v>127.96236213319979</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3698,22 +3698,22 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>0.6578403253678454</v>
+        <v>0.5607497759758528</v>
       </c>
       <c r="C25">
-        <v>110.4281189656015</v>
+        <v>112.0818169026329</v>
       </c>
       <c r="D25">
-        <v>0.5653556535364932</v>
+        <v>0.33217132839129626</v>
       </c>
       <c r="E25">
-        <v>18.939209523738118</v>
+        <v>17.732743551485967</v>
       </c>
       <c r="F25">
-        <v>0.09893865332712266</v>
+        <v>0.0700672874293736</v>
       </c>
       <c r="G25">
-        <v>129.47351856736609</v>
+        <v>129.48839198944663</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3721,22 +3721,22 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>0.6694893203272386</v>
+        <v>0.6381733537478024</v>
       </c>
       <c r="C26">
-        <v>108.51071229196042</v>
+        <v>110.24773579425052</v>
       </c>
       <c r="D26">
-        <v>0.6250204168273392</v>
+        <v>0.36985149776339216</v>
       </c>
       <c r="E26">
-        <v>19.260235496935874</v>
+        <v>18.09787327008998</v>
       </c>
       <c r="F26">
-        <v>0.20686617203133476</v>
+        <v>0.1076336806101934</v>
       </c>
       <c r="G26">
-        <v>128.94106806442682</v>
+        <v>128.71286412797954</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3744,22 +3744,22 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>0.36945367588515826</v>
+        <v>0.30907382805390726</v>
       </c>
       <c r="C27">
-        <v>97.98824442881168</v>
+        <v>100.4297195046533</v>
       </c>
       <c r="D27">
-        <v>0.9615308148654725</v>
+        <v>0.7157339171401162</v>
       </c>
       <c r="E27">
-        <v>16.440722709630208</v>
+        <v>15.775000090562363</v>
       </c>
       <c r="F27">
-        <v>0.043329207253469545</v>
+        <v>0.03428475320077747</v>
       </c>
       <c r="G27">
-        <v>124.55843456153404</v>
+        <v>125.01618764549538</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3767,22 +3767,22 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>0.1641257396295878</v>
+        <v>0.24810223169958773</v>
       </c>
       <c r="C28">
-        <v>101.04955962996488</v>
+        <v>103.58920393865442</v>
       </c>
       <c r="D28">
-        <v>0.6197987596311448</v>
+        <v>0.6282900802931483</v>
       </c>
       <c r="E28">
-        <v>19.32201405204778</v>
+        <v>18.166382730935997</v>
       </c>
       <c r="F28">
-        <v>0.01360647151942501</v>
+        <v>0.02621935692557715</v>
       </c>
       <c r="G28">
-        <v>125.15459450583856</v>
+        <v>125.59272304465765</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3790,22 +3790,22 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>0.2463989723960163</v>
+        <v>0.3526207593837022</v>
       </c>
       <c r="C29">
-        <v>103.97959244998299</v>
+        <v>106.62187633761592</v>
       </c>
       <c r="D29">
-        <v>0.7447715621741567</v>
+        <v>0.756130227206642</v>
       </c>
       <c r="E29">
-        <v>21.58052626476842</v>
+        <v>20.32943828581663</v>
       </c>
       <c r="F29">
-        <v>0.02722792873808198</v>
+        <v>0.04312260111639292</v>
       </c>
       <c r="G29">
-        <v>125.71381734875109</v>
+        <v>126.12190633903812</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3813,22 +3813,22 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>0.23315476807001753</v>
+        <v>0.32750060197594616</v>
       </c>
       <c r="C30">
-        <v>121.76233570730516</v>
+        <v>124.29347914338241</v>
       </c>
       <c r="D30">
-        <v>0.7435644281929789</v>
+        <v>0.7556863241173551</v>
       </c>
       <c r="E30">
-        <v>15.79284348013266</v>
+        <v>14.752879068483471</v>
       </c>
       <c r="F30">
-        <v>0.03996719231544301</v>
+        <v>0.07043876170449169</v>
       </c>
       <c r="G30">
-        <v>127.6768684546037</v>
+        <v>127.99669043113988</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3836,22 +3836,22 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>0.29244119980296956</v>
+        <v>0.3832942219450052</v>
       </c>
       <c r="C31">
-        <v>120.10535474019402</v>
+        <v>122.60795440652244</v>
       </c>
       <c r="D31">
-        <v>0.8157988913877546</v>
+        <v>0.8217830113812545</v>
       </c>
       <c r="E31">
-        <v>16.25655578158666</v>
+        <v>15.160113003813787</v>
       </c>
       <c r="F31">
-        <v>0.05704788873147013</v>
+        <v>0.09904787058459484</v>
       </c>
       <c r="G31">
-        <v>126.69353873777094</v>
+        <v>127.08980621488564</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3859,22 +3859,22 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>0.1822120096995416</v>
+        <v>0.3625465880381993</v>
       </c>
       <c r="C32">
-        <v>108.79061017906619</v>
+        <v>111.33674616211843</v>
       </c>
       <c r="D32">
-        <v>0.8779363374162614</v>
+        <v>0.7554550245267118</v>
       </c>
       <c r="E32">
-        <v>14.227133814343855</v>
+        <v>13.323089191646215</v>
       </c>
       <c r="F32">
-        <v>0.03533505164498108</v>
+        <v>0.10220378406915696</v>
       </c>
       <c r="G32">
-        <v>121.71398380438144</v>
+        <v>122.3814451380828</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3882,22 +3882,22 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>0.18763864024522733</v>
+        <v>0.23138716394240977</v>
       </c>
       <c r="C33">
-        <v>112.11826783211589</v>
+        <v>114.7528281724591</v>
       </c>
       <c r="D33">
-        <v>0.8800234735964654</v>
+        <v>0.5601013424349467</v>
       </c>
       <c r="E33">
-        <v>16.11469312033304</v>
+        <v>15.552891210777904</v>
       </c>
       <c r="F33">
-        <v>0.037509785837174785</v>
+        <v>0.04789109006916713</v>
       </c>
       <c r="G33">
-        <v>122.39954764386455</v>
+        <v>123.04621953647165</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3905,22 +3905,22 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>0.011884189764610935</v>
+        <v>0.20236487017591717</v>
       </c>
       <c r="C34">
-        <v>114.76083974792115</v>
+        <v>117.60449231375604</v>
       </c>
       <c r="D34">
-        <v>1.04524386148472</v>
+        <v>0.6701280658416608</v>
       </c>
       <c r="E34">
-        <v>17.897150236863475</v>
+        <v>17.32636676556264</v>
       </c>
       <c r="F34">
-        <v>0.30219095009647945</v>
+        <v>0.17790396847562245</v>
       </c>
       <c r="G34">
-        <v>124.58116385137428</v>
+        <v>124.7444861415173</v>
       </c>
     </row>
   </sheetData>
@@ -3989,22 +3989,22 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>0.8259075909628004</v>
+        <v>0.8214932130097187</v>
       </c>
       <c r="C5">
-        <v>0.22651787250311695</v>
+        <v>0.23093225045619892</v>
       </c>
       <c r="D5">
-        <v>0.21710788570615977</v>
+        <v>0.21710788570615974</v>
       </c>
       <c r="E5">
-        <v>0.6607260727702401</v>
+        <v>0.6571945704077745</v>
       </c>
       <c r="F5">
-        <v>0.18121429800249356</v>
+        <v>0.1847458003649592</v>
       </c>
       <c r="G5">
-        <v>0.19973925484966626</v>
+        <v>0.19973925484966634</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4012,22 +4012,22 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>0.6748823930799471</v>
+        <v>0.6703404949901575</v>
       </c>
       <c r="C6">
-        <v>0.18786972518063333</v>
+        <v>0.1926521699364764</v>
       </c>
       <c r="D6">
-        <v>0.19560794505116855</v>
+        <v>0.19980810258812015</v>
       </c>
       <c r="E6">
-        <v>0.5399059144639572</v>
+        <v>0.5362723959921254</v>
       </c>
       <c r="F6">
-        <v>0.15029578014450665</v>
+        <v>0.1541217359491812</v>
       </c>
       <c r="G6">
-        <v>0.17995930944707453</v>
+        <v>0.1838234543810719</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4035,22 +4035,22 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>0.6828658488885798</v>
+        <v>0.6786170928985046</v>
       </c>
       <c r="C7">
-        <v>0.19065956809491663</v>
+        <v>0.19515716583504275</v>
       </c>
       <c r="D7">
-        <v>0.1987916286493786</v>
+        <v>0.20282075360052762</v>
       </c>
       <c r="E7">
-        <v>0.5462926791108633</v>
+        <v>0.5428936743188034</v>
       </c>
       <c r="F7">
-        <v>0.15252765447593333</v>
+        <v>0.1561257326680342</v>
       </c>
       <c r="G7">
-        <v>0.18288829835742781</v>
+        <v>0.18659509331248678</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4058,22 +4058,22 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>0.6114972611212726</v>
+        <v>0.640315263204683</v>
       </c>
       <c r="C8">
-        <v>0.1737092989249779</v>
+        <v>0.18507109493217988</v>
       </c>
       <c r="D8">
-        <v>0.18007870996834127</v>
+        <v>0.19182799356631797</v>
       </c>
       <c r="E8">
-        <v>0.48919780889701797</v>
+        <v>0.5122522105637464</v>
       </c>
       <c r="F8">
-        <v>0.13896743913998233</v>
+        <v>0.1480568759457439</v>
       </c>
       <c r="G8">
-        <v>0.16567241317087347</v>
+        <v>0.1764817540810136</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4081,22 +4081,22 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>0.6241038555585505</v>
+        <v>0.653971887862478</v>
       </c>
       <c r="C9">
-        <v>0.17619298287618362</v>
+        <v>0.1874381454339324</v>
       </c>
       <c r="D9">
-        <v>0.18290662134779262</v>
+        <v>0.19312391311544125</v>
       </c>
       <c r="E9">
-        <v>0.4992830844468405</v>
+        <v>0.5231775102899824</v>
       </c>
       <c r="F9">
-        <v>0.14095438630094695</v>
+        <v>0.1499505163471459</v>
       </c>
       <c r="G9">
-        <v>0.1682740916399688</v>
+        <v>0.1776740000662072</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4104,22 +4104,22 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>0.6621766181965069</v>
+        <v>0.6892270384071348</v>
       </c>
       <c r="C10">
-        <v>0.18033639359553696</v>
+        <v>0.1942300516187841</v>
       </c>
       <c r="D10">
-        <v>0.19926567779867918</v>
+        <v>0.2132615926546026</v>
       </c>
       <c r="E10">
-        <v>0.5297412945572051</v>
+        <v>0.5513816307257081</v>
       </c>
       <c r="F10">
-        <v>0.1442691148764296</v>
+        <v>0.15538404129502734</v>
       </c>
       <c r="G10">
-        <v>0.18332442357478435</v>
+        <v>0.19620066524223595</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4127,22 +4127,22 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>0.65324106023405</v>
+        <v>0.6812430396425193</v>
       </c>
       <c r="C11">
-        <v>0.17913051847439015</v>
+        <v>0.19135209880156728</v>
       </c>
       <c r="D11">
-        <v>0.1970145842621571</v>
+        <v>0.21016800971200766</v>
       </c>
       <c r="E11">
-        <v>0.52259284818724</v>
+        <v>0.5449944317140153</v>
       </c>
       <c r="F11">
-        <v>0.14330441477951208</v>
+        <v>0.15308167904125383</v>
       </c>
       <c r="G11">
-        <v>0.18125341752118404</v>
+        <v>0.19335456893504835</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4150,22 +4150,22 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>0.6446209341136002</v>
+        <v>0.671550996892811</v>
       </c>
       <c r="C12">
-        <v>0.17782426480252486</v>
+        <v>0.18836309607932983</v>
       </c>
       <c r="D12">
-        <v>0.19499332250691945</v>
+        <v>0.2073263707280339</v>
       </c>
       <c r="E12">
-        <v>0.5156967472908791</v>
+        <v>0.5372407975142491</v>
       </c>
       <c r="F12">
-        <v>0.14225941184201985</v>
+        <v>0.1506904768634639</v>
       </c>
       <c r="G12">
-        <v>0.1793938567063653</v>
+        <v>0.19074026106979272</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4173,22 +4173,22 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>0.6420999901690336</v>
+        <v>0.6637716724227667</v>
       </c>
       <c r="C13">
-        <v>0.17678017724194325</v>
+        <v>0.1865666453918697</v>
       </c>
       <c r="D13">
-        <v>0.19320441137508843</v>
+        <v>0.20480740216692161</v>
       </c>
       <c r="E13">
-        <v>0.513679992135227</v>
+        <v>0.5310173379382133</v>
       </c>
       <c r="F13">
-        <v>0.1414241417935546</v>
+        <v>0.14925331631349584</v>
       </c>
       <c r="G13">
-        <v>0.17774805846508085</v>
+        <v>0.18842280999356928</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4196,22 +4196,22 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>0.6384395320411661</v>
+        <v>0.6572686866005085</v>
       </c>
       <c r="C14">
-        <v>0.17517716896542831</v>
+        <v>0.18436217002588356</v>
       </c>
       <c r="D14">
-        <v>0.18857122803882964</v>
+        <v>0.20243196181430595</v>
       </c>
       <c r="E14">
-        <v>0.5107516256329329</v>
+        <v>0.5258149492804067</v>
       </c>
       <c r="F14">
-        <v>0.14014173517234266</v>
+        <v>0.1474897360207069</v>
       </c>
       <c r="G14">
-        <v>0.17348552979572274</v>
+        <v>0.1862374048691628</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4219,22 +4219,22 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>0.8641288939322233</v>
+        <v>0.8550927002065757</v>
       </c>
       <c r="C15">
-        <v>0.23744776628839345</v>
+        <v>0.24328491050308385</v>
       </c>
       <c r="D15">
-        <v>0.0</v>
+        <v>0.0022318162217492376</v>
       </c>
       <c r="E15">
-        <v>0.6913031151457776</v>
+        <v>0.6840741601652608</v>
       </c>
       <c r="F15">
-        <v>0.18995821303071472</v>
+        <v>0.19462792840246698</v>
       </c>
       <c r="G15">
-        <v>0.0</v>
+        <v>0.0020532709240093107</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4242,22 +4242,22 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>0.8565519080364377</v>
+        <v>0.8570911327701729</v>
       </c>
       <c r="C16">
-        <v>0.24042779708999074</v>
+        <v>0.24395758645155832</v>
       </c>
       <c r="D16">
-        <v>0.0</v>
+        <v>0.009989600180633787</v>
       </c>
       <c r="E16">
-        <v>0.6852415264291504</v>
+        <v>0.6856729062161389</v>
       </c>
       <c r="F16">
-        <v>0.19234223767199263</v>
+        <v>0.19516606916124665</v>
       </c>
       <c r="G16">
-        <v>0.0</v>
+        <v>0.009190432166183031</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4265,22 +4265,22 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>0.8487825561641716</v>
+        <v>0.8569011040135989</v>
       </c>
       <c r="C17">
-        <v>0.23771996577023383</v>
+        <v>0.2422730336377708</v>
       </c>
       <c r="D17">
-        <v>0.0</v>
+        <v>0.009975616504091823</v>
       </c>
       <c r="E17">
-        <v>0.679026044931337</v>
+        <v>0.6855208832108795</v>
       </c>
       <c r="F17">
-        <v>0.19017597261618696</v>
+        <v>0.19381842691021667</v>
       </c>
       <c r="G17">
-        <v>0.0</v>
+        <v>0.009177567183764425</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4288,22 +4288,22 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>0.8349836105812825</v>
+        <v>0.8437372782747793</v>
       </c>
       <c r="C18">
-        <v>0.22926117002454913</v>
+        <v>0.2382999542025053</v>
       </c>
       <c r="D18">
-        <v>0.0</v>
+        <v>0.00985191073075971</v>
       </c>
       <c r="E18">
-        <v>0.6679868884650262</v>
+        <v>0.6749898226198234</v>
       </c>
       <c r="F18">
-        <v>0.1834089360196393</v>
+        <v>0.19063996336200423</v>
       </c>
       <c r="G18">
-        <v>0.0</v>
+        <v>0.009063757872298881</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4311,22 +4311,22 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>0.8199521616490035</v>
+        <v>0.8335032728897043</v>
       </c>
       <c r="C19">
-        <v>0.22549570778354974</v>
+        <v>0.2309790128931975</v>
       </c>
       <c r="D19">
-        <v>0.0</v>
+        <v>0.009729514415740522</v>
       </c>
       <c r="E19">
-        <v>0.655961729319203</v>
+        <v>0.6668026183117632</v>
       </c>
       <c r="F19">
-        <v>0.1803965662268398</v>
+        <v>0.18478321031455797</v>
       </c>
       <c r="G19">
-        <v>0.0</v>
+        <v>0.008951153262481228</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4334,22 +4334,22 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>0.8000321797737816</v>
+        <v>0.7930937948266541</v>
       </c>
       <c r="C20">
-        <v>0.2241706766648045</v>
+        <v>0.2260686181441196</v>
       </c>
       <c r="D20">
-        <v>0.0</v>
+        <v>0.009024864576550173</v>
       </c>
       <c r="E20">
-        <v>0.640025743819025</v>
+        <v>0.6344750358613238</v>
       </c>
       <c r="F20">
-        <v>0.17933654133184362</v>
+        <v>0.18085489451529566</v>
       </c>
       <c r="G20">
-        <v>0.0</v>
+        <v>0.00830287541042614</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4357,22 +4357,22 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>0.8068460007942442</v>
+        <v>0.8028613446344238</v>
       </c>
       <c r="C21">
-        <v>0.22959522970623192</v>
+        <v>0.23098077506152084</v>
       </c>
       <c r="D21">
-        <v>0.0</v>
+        <v>0.007105238475941884</v>
       </c>
       <c r="E21">
-        <v>0.6454768006353951</v>
+        <v>0.6422890757075397</v>
       </c>
       <c r="F21">
-        <v>0.1836761837649856</v>
+        <v>0.18478462004921667</v>
       </c>
       <c r="G21">
-        <v>0.0</v>
+        <v>0.006536819397866551</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4380,22 +4380,22 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>0.8166008966229649</v>
+        <v>0.8124728001181039</v>
       </c>
       <c r="C22">
-        <v>0.22960005712564607</v>
+        <v>0.23207009065618486</v>
       </c>
       <c r="D22">
-        <v>0.0</v>
+        <v>0.007292446306286198</v>
       </c>
       <c r="E22">
-        <v>0.6532807172983722</v>
+        <v>0.649978240094483</v>
       </c>
       <c r="F22">
-        <v>0.18368004570051688</v>
+        <v>0.18565607252494787</v>
       </c>
       <c r="G22">
-        <v>0.0</v>
+        <v>0.006709050601783316</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4403,22 +4403,22 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>0.8125012060105963</v>
+        <v>0.80684590106882</v>
       </c>
       <c r="C23">
-        <v>0.2296818938655498</v>
+        <v>0.23041614089595863</v>
       </c>
       <c r="D23">
-        <v>0.0</v>
+        <v>0.007109826186748404</v>
       </c>
       <c r="E23">
-        <v>0.6500009648084766</v>
+        <v>0.6454767208550558</v>
       </c>
       <c r="F23">
-        <v>0.1837455150924399</v>
+        <v>0.18433291271676688</v>
       </c>
       <c r="G23">
-        <v>0.0</v>
+        <v>0.006541040091808543</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4426,22 +4426,22 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>0.8266413766620692</v>
+        <v>0.8152146873996584</v>
       </c>
       <c r="C24">
-        <v>0.23391801369427076</v>
+        <v>0.23077379472250142</v>
       </c>
       <c r="D24">
-        <v>0.0</v>
+        <v>0.0071897359629814386</v>
       </c>
       <c r="E24">
-        <v>0.6613131013296554</v>
+        <v>0.6521717499197272</v>
       </c>
       <c r="F24">
-        <v>0.18713441095541658</v>
+        <v>0.18461903577800118</v>
       </c>
       <c r="G24">
-        <v>0.0</v>
+        <v>0.006614557085942943</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4449,22 +4449,22 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>0.7625429331753633</v>
+        <v>0.7385509079139017</v>
       </c>
       <c r="C25">
-        <v>0.21808131287643545</v>
+        <v>0.21552106810484173</v>
       </c>
       <c r="D25">
-        <v>0.0</v>
+        <v>0.0065712026625412345</v>
       </c>
       <c r="E25">
-        <v>0.610034346540291</v>
+        <v>0.5908407263311218</v>
       </c>
       <c r="F25">
-        <v>0.17446505030114834</v>
+        <v>0.17241685448387342</v>
       </c>
       <c r="G25">
-        <v>0.0</v>
+        <v>0.006045506449537948</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4472,22 +4472,22 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>0.7816674703950781</v>
+        <v>0.7497544177138138</v>
       </c>
       <c r="C26">
-        <v>0.2214252639949303</v>
+        <v>0.2169752385297407</v>
       </c>
       <c r="D26">
-        <v>0.0</v>
+        <v>0.006771453854596162</v>
       </c>
       <c r="E26">
-        <v>0.6253339763160626</v>
+        <v>0.5998035341710515</v>
       </c>
       <c r="F26">
-        <v>0.17714021119594417</v>
+        <v>0.17358019082379259</v>
       </c>
       <c r="G26">
-        <v>0.0</v>
+        <v>0.0062297375462284825</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -4495,22 +4495,22 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>0.7818843606322876</v>
+        <v>0.7599608545406781</v>
       </c>
       <c r="C27">
-        <v>0.21883212180829553</v>
+        <v>0.21634628268909045</v>
       </c>
       <c r="D27">
-        <v>0.0</v>
+        <v>0.00735886714382646</v>
       </c>
       <c r="E27">
-        <v>0.6255074885058304</v>
+        <v>0.6079686836325422</v>
       </c>
       <c r="F27">
-        <v>0.17506569744663641</v>
+        <v>0.17307702615127235</v>
       </c>
       <c r="G27">
-        <v>0.0</v>
+        <v>0.006770157772320365</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -4518,22 +4518,22 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>0.7865513460989046</v>
+        <v>0.7737426548282649</v>
       </c>
       <c r="C28">
-        <v>0.22005722929134447</v>
+        <v>0.21898612829245548</v>
       </c>
       <c r="D28">
-        <v>0.0</v>
+        <v>0.0073387058639803595</v>
       </c>
       <c r="E28">
-        <v>0.6292410768791237</v>
+        <v>0.6189941238626123</v>
       </c>
       <c r="F28">
-        <v>0.17604578343307553</v>
+        <v>0.1751889026339644</v>
       </c>
       <c r="G28">
-        <v>0.0</v>
+        <v>0.00675160939486195</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -4541,22 +4541,22 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>0.7885648718901332</v>
+        <v>0.7803439264205637</v>
       </c>
       <c r="C29">
-        <v>0.22106920029475938</v>
+        <v>0.22117848285200864</v>
       </c>
       <c r="D29">
-        <v>0.0</v>
+        <v>0.0072541724977685015</v>
       </c>
       <c r="E29">
-        <v>0.6308518975121068</v>
+        <v>0.6242751411364511</v>
       </c>
       <c r="F29">
-        <v>0.17685536023580742</v>
+        <v>0.17694278628160695</v>
       </c>
       <c r="G29">
-        <v>0.0</v>
+        <v>0.006673838697947043</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4564,22 +4564,22 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>0.7073780219392636</v>
+        <v>0.6815180489278545</v>
       </c>
       <c r="C30">
-        <v>0.19910573823236213</v>
+        <v>0.19560738047362528</v>
       </c>
       <c r="D30">
-        <v>0.0</v>
+        <v>0.006442672674534945</v>
       </c>
       <c r="E30">
-        <v>0.5659024175514107</v>
+        <v>0.5452144391422837</v>
       </c>
       <c r="F30">
-        <v>0.1592845905858897</v>
+        <v>0.15648590437890023</v>
       </c>
       <c r="G30">
-        <v>0.0</v>
+        <v>0.005927258860572165</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4587,22 +4587,22 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>0.7195361832929923</v>
+        <v>0.70443377390364</v>
       </c>
       <c r="C31">
-        <v>0.2032313549441349</v>
+        <v>0.1983736855174651</v>
       </c>
       <c r="D31">
-        <v>0.0</v>
+        <v>0.061599974559944204</v>
       </c>
       <c r="E31">
-        <v>0.5756289466343938</v>
+        <v>0.5635470191229118</v>
       </c>
       <c r="F31">
-        <v>0.1625850839553079</v>
+        <v>0.1586989484139721</v>
       </c>
       <c r="G31">
-        <v>0.0</v>
+        <v>0.056671976595148096</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -4610,22 +4610,22 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>0.7299894929446618</v>
+        <v>0.717929613326634</v>
       </c>
       <c r="C32">
-        <v>0.20253676582025232</v>
+        <v>0.2020983116935325</v>
       </c>
       <c r="D32">
-        <v>0.0</v>
+        <v>0.06891571555436822</v>
       </c>
       <c r="E32">
-        <v>0.5839915943557298</v>
+        <v>0.5743436906613069</v>
       </c>
       <c r="F32">
-        <v>0.16202941265620183</v>
+        <v>0.161678649354826</v>
       </c>
       <c r="G32">
-        <v>0.0</v>
+        <v>0.0634024583100184</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -4633,22 +4633,22 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>0.7494956974834317</v>
+        <v>0.7283556309598215</v>
       </c>
       <c r="C33">
-        <v>0.2091409353067449</v>
+        <v>0.2042618083578893</v>
       </c>
       <c r="D33">
-        <v>0.0</v>
+        <v>0.06870536937976378</v>
       </c>
       <c r="E33">
-        <v>0.5995965579867456</v>
+        <v>0.5826845047678568</v>
       </c>
       <c r="F33">
-        <v>0.16731274824539594</v>
+        <v>0.16340944668631135</v>
       </c>
       <c r="G33">
-        <v>0.0</v>
+        <v>0.06320893982938228</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -4656,22 +4656,22 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>0.7795972265780089</v>
+        <v>0.768149938322864</v>
       </c>
       <c r="C34">
-        <v>0.2233127486167252</v>
+        <v>0.21559701579774235</v>
       </c>
       <c r="D34">
-        <v>0.0</v>
+        <v>0.07398362697944211</v>
       </c>
       <c r="E34">
-        <v>0.6236777812624064</v>
+        <v>0.6145199506582913</v>
       </c>
       <c r="F34">
-        <v>0.17865019889338024</v>
+        <v>0.17247761263819392</v>
       </c>
       <c r="G34">
-        <v>0.0</v>
+        <v>0.06806493682108662</v>
       </c>
     </row>
   </sheetData>
@@ -4736,13 +4736,13 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>67.49226369721264</v>
+        <v>67.55351554567446</v>
       </c>
       <c r="C6">
-        <v>11.08916339999999</v>
+        <v>11.028318338550722</v>
       </c>
       <c r="D6">
-        <v>4.910476449999997</v>
+        <v>4.910470399999997</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4750,13 +4750,13 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>67.49941213335848</v>
+        <v>67.56981114821124</v>
       </c>
       <c r="C7">
-        <v>11.08916339999999</v>
+        <v>11.019260825789553</v>
       </c>
       <c r="D7">
-        <v>4.910476449999997</v>
+        <v>4.91034904981847</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4764,13 +4764,13 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>67.50740341493277</v>
+        <v>67.56953339846105</v>
       </c>
       <c r="C8">
-        <v>11.08916339999999</v>
+        <v>11.028573316985272</v>
       </c>
       <c r="D8">
-        <v>4.910476449999997</v>
+        <v>4.909384120493969</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4778,13 +4778,13 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>67.51499514783004</v>
+        <v>67.57871536967824</v>
       </c>
       <c r="C9">
-        <v>11.08916339999999</v>
+        <v>11.027427931516337</v>
       </c>
       <c r="D9">
-        <v>4.910476449999997</v>
+        <v>4.908862025233368</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4792,13 +4792,13 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>67.49611445652734</v>
+        <v>67.57444543956105</v>
       </c>
       <c r="C10">
-        <v>11.08916339999999</v>
+        <v>11.016737531659166</v>
       </c>
       <c r="D10">
-        <v>4.017662550000014</v>
+        <v>4.017270882794058</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4806,13 +4806,13 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>67.50163220345638</v>
+        <v>67.57600460264405</v>
       </c>
       <c r="C11">
-        <v>11.08916339999999</v>
+        <v>11.020449085172812</v>
       </c>
       <c r="D11">
-        <v>4.017662550000014</v>
+        <v>4.017184951567218</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4820,13 +4820,13 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>67.50765855653763</v>
+        <v>67.5741666447366</v>
       </c>
       <c r="C12">
-        <v>11.08916339999999</v>
+        <v>11.028031843137017</v>
       </c>
       <c r="D12">
-        <v>4.017662550000014</v>
+        <v>4.017096320340378</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4834,13 +4834,13 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>67.51397742502192</v>
+        <v>67.57763720462019</v>
       </c>
       <c r="C13">
-        <v>11.08916339999999</v>
+        <v>11.030319727142503</v>
       </c>
       <c r="D13">
-        <v>4.017662550000014</v>
+        <v>4.0172806522160025</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4848,13 +4848,13 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>67.51981701154902</v>
+        <v>67.58004518211746</v>
       </c>
       <c r="C14">
-        <v>11.08916339999999</v>
+        <v>11.033355101817166</v>
       </c>
       <c r="D14">
-        <v>4.017662550000014</v>
+        <v>4.017399290679525</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4862,13 +4862,13 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>67.54308808702183</v>
+        <v>67.58501047325801</v>
       </c>
       <c r="C15">
-        <v>11.08916339999999</v>
+        <v>11.047410196559435</v>
       </c>
       <c r="D15">
-        <v>2.23203475</v>
+        <v>2.2319586311601185</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4876,13 +4876,13 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>67.5563541343866</v>
+        <v>67.58977236118457</v>
       </c>
       <c r="C16">
-        <v>11.08916339999999</v>
+        <v>11.056581921672246</v>
       </c>
       <c r="D16">
-        <v>2.23203475</v>
+        <v>2.231987</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4890,13 +4890,13 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>67.56810791708715</v>
+        <v>67.5900346408402</v>
       </c>
       <c r="C17">
-        <v>11.092760785674532</v>
+        <v>12.767698012417966</v>
       </c>
       <c r="D17">
-        <v>2.23203475</v>
+        <v>2.231987</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4904,13 +4904,13 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>67.57489113080511</v>
+        <v>67.59492327573925</v>
       </c>
       <c r="C18">
-        <v>11.092760785674532</v>
+        <v>12.773042640620938</v>
       </c>
       <c r="D18">
-        <v>2.23203475</v>
+        <v>2.2320125</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4918,13 +4918,13 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>67.43307690870782</v>
+        <v>67.5976846257678</v>
       </c>
       <c r="C19">
-        <v>11.09079664097786</v>
+        <v>12.777824215670028</v>
       </c>
       <c r="D19">
-        <v>2.23203475</v>
+        <v>2.23201775</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4932,10 +4932,10 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>67.58731125862501</v>
+        <v>67.5991118711479</v>
       </c>
       <c r="C20">
-        <v>11.092760785674532</v>
+        <v>12.782605304244209</v>
       </c>
       <c r="D20">
         <v>0.0</v>
@@ -4946,10 +4946,10 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>67.59172117792117</v>
+        <v>67.60228690058223</v>
       </c>
       <c r="C21">
-        <v>11.092760785674532</v>
+        <v>12.78500190276291</v>
       </c>
       <c r="D21">
         <v>0.0</v>
@@ -4960,10 +4960,10 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>67.55616306700377</v>
+        <v>67.5933716768676</v>
       </c>
       <c r="C22">
-        <v>20.539627564055603</v>
+        <v>20.39788708207092</v>
       </c>
       <c r="D22">
         <v>0.0</v>
@@ -4974,10 +4974,10 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>67.56456515801108</v>
+        <v>67.59272523307143</v>
       </c>
       <c r="C23">
-        <v>20.539627564055603</v>
+        <v>20.40679461595517</v>
       </c>
       <c r="D23">
         <v>0.0</v>
@@ -4988,10 +4988,10 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>67.38529784422467</v>
+        <v>67.59595206330695</v>
       </c>
       <c r="C24">
-        <v>20.53258503094198</v>
+        <v>20.411434597909878</v>
       </c>
       <c r="D24">
         <v>0.0</v>
@@ -5002,10 +5002,10 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>59.48656762088007</v>
+        <v>59.493246840688265</v>
       </c>
       <c r="C25">
-        <v>20.539627564055603</v>
+        <v>20.427743545200382</v>
       </c>
       <c r="D25">
         <v>0.0</v>
@@ -5016,10 +5016,10 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>67.44298117590145</v>
+        <v>67.6004688887764</v>
       </c>
       <c r="C26">
-        <v>20.53909208190718</v>
+        <v>20.417862244168987</v>
       </c>
       <c r="D26">
         <v>0.0</v>
@@ -5030,10 +5030,10 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>67.32026464735345</v>
+        <v>67.51743385594541</v>
       </c>
       <c r="C27">
-        <v>44.51751392769135</v>
+        <v>42.39840776233839</v>
       </c>
       <c r="D27">
         <v>0.0</v>
@@ -5044,10 +5044,10 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>67.36006722576269</v>
+        <v>67.531201733683</v>
       </c>
       <c r="C28">
-        <v>44.5175464016096</v>
+        <v>42.417000807166545</v>
       </c>
       <c r="D28">
         <v>0.0</v>
@@ -5058,10 +5058,10 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>67.39200433337521</v>
+        <v>67.53251206949538</v>
       </c>
       <c r="C29">
-        <v>44.51757887552785</v>
+        <v>42.44304643435265</v>
       </c>
       <c r="D29">
         <v>0.0</v>
@@ -5072,10 +5072,10 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>59.41397656537126</v>
+        <v>59.468135116133226</v>
       </c>
       <c r="C30">
-        <v>44.51818441198558</v>
+        <v>42.510034371464606</v>
       </c>
       <c r="D30">
         <v>0.0</v>
@@ -5086,10 +5086,10 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>67.44560198012105</v>
+        <v>67.55397758399509</v>
       </c>
       <c r="C31">
-        <v>44.51818441198558</v>
+        <v>42.466076821993774</v>
       </c>
       <c r="D31">
         <v>0.0</v>
@@ -5100,10 +5100,10 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>66.72568449383552</v>
+        <v>67.28518854310398</v>
       </c>
       <c r="C32">
-        <v>69.63360003369185</v>
+        <v>66.63748796622382</v>
       </c>
       <c r="D32">
         <v>0.0</v>
@@ -5114,10 +5114,10 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>66.81989220335561</v>
+        <v>67.30660594430638</v>
       </c>
       <c r="C33">
-        <v>69.6341449498882</v>
+        <v>66.69272955384331</v>
       </c>
       <c r="D33">
         <v>0.0</v>
@@ -5128,10 +5128,10 @@
         <v>2049</v>
       </c>
       <c r="B34">
-        <v>66.00274969574203</v>
+        <v>67.04679831428945</v>
       </c>
       <c r="C34">
-        <v>69.59291716411563</v>
+        <v>66.42665365457138</v>
       </c>
       <c r="D34">
         <v>0.0</v>
@@ -5179,7 +5179,7 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>67.8072781992243</v>
+        <v>67.80727819922357</v>
       </c>
       <c r="C5">
         <v>-0.0</v>
@@ -5190,7 +5190,7 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>46.16948226057717</v>
+        <v>46.16766902687382</v>
       </c>
       <c r="C6">
         <v>-0.0</v>
@@ -5201,7 +5201,7 @@
         <v>2022</v>
       </c>
       <c r="B7">
-        <v>47.05957498891443</v>
+        <v>47.05749375611664</v>
       </c>
       <c r="C7">
         <v>-0.0</v>
@@ -5212,7 +5212,7 @@
         <v>2023</v>
       </c>
       <c r="B8">
-        <v>46.798353984439196</v>
+        <v>47.162820709210536</v>
       </c>
       <c r="C8">
         <v>-0.0</v>
@@ -5223,7 +5223,7 @@
         <v>2024</v>
       </c>
       <c r="B9">
-        <v>47.66122266334186</v>
+        <v>48.04028565062916</v>
       </c>
       <c r="C9">
         <v>-0.0</v>
@@ -5234,7 +5234,7 @@
         <v>2025</v>
       </c>
       <c r="B10">
-        <v>18.1176211848974</v>
+        <v>17.487416175426194</v>
       </c>
       <c r="C10">
         <v>-0.0</v>
@@ -5245,7 +5245,7 @@
         <v>2026</v>
       </c>
       <c r="B11">
-        <v>18.679169257445775</v>
+        <v>18.040099218364848</v>
       </c>
       <c r="C11">
         <v>-0.0</v>
@@ -5256,7 +5256,7 @@
         <v>2027</v>
       </c>
       <c r="B12">
-        <v>19.24814911297695</v>
+        <v>18.600770025834805</v>
       </c>
       <c r="C12">
         <v>-0.0</v>
@@ -5267,7 +5267,7 @@
         <v>2028</v>
       </c>
       <c r="B13">
-        <v>19.824868930054855</v>
+        <v>19.169579381289175</v>
       </c>
       <c r="C13">
         <v>-0.0</v>
@@ -5278,7 +5278,7 @@
         <v>2029</v>
       </c>
       <c r="B14">
-        <v>20.40910603391831</v>
+        <v>19.745796636188995</v>
       </c>
       <c r="C14">
         <v>-0.0</v>
@@ -5289,7 +5289,7 @@
         <v>2030</v>
       </c>
       <c r="B15">
-        <v>14.105803649362626</v>
+        <v>13.630915014368677</v>
       </c>
       <c r="C15">
         <v>-0.0</v>
@@ -5300,7 +5300,7 @@
         <v>2031</v>
       </c>
       <c r="B16">
-        <v>15.501199026887853</v>
+        <v>14.989212567665211</v>
       </c>
       <c r="C16">
         <v>-0.0</v>
@@ -5311,7 +5311,7 @@
         <v>2032</v>
       </c>
       <c r="B17">
-        <v>16.970498371111464</v>
+        <v>16.13351286942242</v>
       </c>
       <c r="C17">
         <v>-0.0</v>
@@ -5322,7 +5322,7 @@
         <v>2033</v>
       </c>
       <c r="B18">
-        <v>18.43699545855146</v>
+        <v>17.497040971169046</v>
       </c>
       <c r="C18">
         <v>-0.0</v>
@@ -5333,10 +5333,10 @@
         <v>2034</v>
       </c>
       <c r="B19">
-        <v>20.0</v>
+        <v>19.027053969923916</v>
       </c>
       <c r="C19">
-        <v>708.5741996233517</v>
+        <v>-0.0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -5344,7 +5344,7 @@
         <v>2035</v>
       </c>
       <c r="B20">
-        <v>16.53642336738266</v>
+        <v>16.206263406225105</v>
       </c>
       <c r="C20">
         <v>-0.0</v>
@@ -5355,7 +5355,7 @@
         <v>2036</v>
       </c>
       <c r="B21">
-        <v>17.93033926878534</v>
+        <v>17.57222176576139</v>
       </c>
       <c r="C21">
         <v>-0.0</v>
@@ -5366,7 +5366,7 @@
         <v>2037</v>
       </c>
       <c r="B22">
-        <v>17.716010310639025</v>
+        <v>17.69287845948593</v>
       </c>
       <c r="C22">
         <v>-0.0</v>
@@ -5377,7 +5377,7 @@
         <v>2038</v>
       </c>
       <c r="B23">
-        <v>18.636063789546405</v>
+        <v>18.562093419300886</v>
       </c>
       <c r="C23">
         <v>-0.0</v>
@@ -5388,10 +5388,10 @@
         <v>2039</v>
       </c>
       <c r="B24">
-        <v>20.0</v>
+        <v>19.95129598589067</v>
       </c>
       <c r="C24">
-        <v>708.5741996233525</v>
+        <v>-0.0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -5399,7 +5399,7 @@
         <v>2040</v>
       </c>
       <c r="B25">
-        <v>19.989786705809536</v>
+        <v>19.54577655054506</v>
       </c>
       <c r="C25">
         <v>-0.0</v>
@@ -5410,10 +5410,10 @@
         <v>2041</v>
       </c>
       <c r="B26">
-        <v>20.0</v>
+        <v>19.57110089709588</v>
       </c>
       <c r="C26">
-        <v>708.574199623352</v>
+        <v>-0.0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -5421,7 +5421,7 @@
         <v>2042</v>
       </c>
       <c r="B27">
-        <v>17.643673760104623</v>
+        <v>17.51235368541524</v>
       </c>
       <c r="C27">
         <v>-0.0</v>
@@ -5432,7 +5432,7 @@
         <v>2043</v>
       </c>
       <c r="B28">
-        <v>18.611526045452997</v>
+        <v>18.589250656923774</v>
       </c>
       <c r="C28">
         <v>-0.0</v>
@@ -5443,7 +5443,7 @@
         <v>2044</v>
       </c>
       <c r="B29">
-        <v>19.859419064327017</v>
+        <v>19.838308940761035</v>
       </c>
       <c r="C29">
         <v>-0.0</v>
@@ -5454,7 +5454,7 @@
         <v>2045</v>
       </c>
       <c r="B30">
-        <v>19.913128032123492</v>
+        <v>19.952846369225526</v>
       </c>
       <c r="C30">
         <v>-0.0</v>
@@ -5465,10 +5465,10 @@
         <v>2046</v>
       </c>
       <c r="B31">
-        <v>19.980377020947138</v>
+        <v>20.0</v>
       </c>
       <c r="C31">
-        <v>-0.0</v>
+        <v>37.26452020202021</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -5476,7 +5476,7 @@
         <v>2047</v>
       </c>
       <c r="B32">
-        <v>17.92048603872539</v>
+        <v>18.035603131155117</v>
       </c>
       <c r="C32">
         <v>-0.0</v>
@@ -5487,7 +5487,7 @@
         <v>2048</v>
       </c>
       <c r="B33">
-        <v>18.952512288547883</v>
+        <v>18.939603986874776</v>
       </c>
       <c r="C33">
         <v>-0.0</v>
@@ -5501,7 +5501,7 @@
         <v>20.0</v>
       </c>
       <c r="C34">
-        <v>7236.55251572327</v>
+        <v>708.5741996233525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>